<commit_message>
filtrages sites ou labos
</commit_message>
<xml_diff>
--- a/Data/FairCarboN_RNSR_copie.xlsx
+++ b/Data/FairCarboN_RNSR_copie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dutroncj\Documents\Outils\FairCarboN_datas\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD23F6DF-BF72-4301-B0C0-D1B8263A8036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{355ADA51-4DA2-4E23-869C-197E5806548D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2886" uniqueCount="1104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2898" uniqueCount="1110">
   <si>
     <t>Titre : Liste des unités du PEPR FairCarboN</t>
   </si>
@@ -3729,14 +3729,32 @@
     <t>Site</t>
   </si>
   <si>
-    <t>Site1</t>
+    <t>Lac Leman</t>
+  </si>
+  <si>
+    <t>Lac Annecy</t>
+  </si>
+  <si>
+    <t>45.874348</t>
+  </si>
+  <si>
+    <t>6.162231</t>
+  </si>
+  <si>
+    <t>Lac Bourget</t>
+  </si>
+  <si>
+    <t>45.697888</t>
+  </si>
+  <si>
+    <t>5.870755</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4163,51 +4181,51 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="13.6328125" customWidth="1"/>
     <col min="3" max="3" width="19.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="43.5">
+    <row r="10" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
@@ -4215,7 +4233,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="58">
+    <row r="12" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="B12" s="7" t="s">
         <v>9</v>
       </c>
@@ -4223,7 +4241,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="29">
+    <row r="13" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="B13" s="8" t="s">
         <v>11</v>
       </c>
@@ -4231,7 +4249,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="43.5">
+    <row r="14" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B14" s="9" t="s">
         <v>13</v>
       </c>
@@ -4239,7 +4257,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -4253,15 +4271,15 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:R187"/>
+  <dimension ref="A1:R189"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="R4" sqref="R4"/>
-      <selection pane="bottomLeft" activeCell="L190" sqref="L190"/>
+      <selection pane="bottomLeft" activeCell="I192" sqref="I192"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.54296875" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.453125" style="10" bestFit="1" customWidth="1"/>
@@ -4284,7 +4302,7 @@
     <col min="19" max="16384" width="8.7265625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="11" customFormat="1">
+    <row r="1" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>16</v>
       </c>
@@ -4340,7 +4358,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="72.5" hidden="1">
+    <row r="2" spans="1:18" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>32</v>
       </c>
@@ -4394,7 +4412,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="58" hidden="1">
+    <row r="3" spans="1:18" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>32</v>
       </c>
@@ -4444,7 +4462,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="174" hidden="1">
+    <row r="4" spans="1:18" ht="174" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>32</v>
       </c>
@@ -4494,7 +4512,7 @@
       </c>
       <c r="R4" s="6"/>
     </row>
-    <row r="5" spans="1:18" ht="87" hidden="1">
+    <row r="5" spans="1:18" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>32</v>
       </c>
@@ -4548,7 +4566,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="145" hidden="1">
+    <row r="6" spans="1:18" ht="145" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>32</v>
       </c>
@@ -4598,7 +4616,7 @@
       <c r="Q6" s="6"/>
       <c r="R6" s="6"/>
     </row>
-    <row r="7" spans="1:18" ht="116" hidden="1">
+    <row r="7" spans="1:18" ht="116" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>32</v>
       </c>
@@ -4650,7 +4668,7 @@
       </c>
       <c r="R7" s="6"/>
     </row>
-    <row r="8" spans="1:18" ht="159.5" hidden="1">
+    <row r="8" spans="1:18" ht="159.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>32</v>
       </c>
@@ -4704,7 +4722,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="87" hidden="1">
+    <row r="9" spans="1:18" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>32</v>
       </c>
@@ -4758,7 +4776,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="116" hidden="1">
+    <row r="10" spans="1:18" ht="116" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>32</v>
       </c>
@@ -4810,7 +4828,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="72.5" hidden="1">
+    <row r="11" spans="1:18" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>32</v>
       </c>
@@ -4864,7 +4882,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="101.5" hidden="1">
+    <row r="12" spans="1:18" ht="101.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>32</v>
       </c>
@@ -4914,7 +4932,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="188.5" hidden="1">
+    <row r="13" spans="1:18" ht="188.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>32</v>
       </c>
@@ -4966,7 +4984,7 @@
       </c>
       <c r="R13" s="6"/>
     </row>
-    <row r="14" spans="1:18" ht="174" hidden="1">
+    <row r="14" spans="1:18" ht="174" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>32</v>
       </c>
@@ -5018,7 +5036,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="101.5" hidden="1">
+    <row r="15" spans="1:18" ht="101.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>32</v>
       </c>
@@ -5066,7 +5084,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="87" hidden="1">
+    <row r="16" spans="1:18" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>32</v>
       </c>
@@ -5118,7 +5136,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="101.5" hidden="1">
+    <row r="17" spans="1:18" ht="101.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
         <v>32</v>
       </c>
@@ -5170,7 +5188,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="58" hidden="1">
+    <row r="18" spans="1:18" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
         <v>32</v>
       </c>
@@ -5222,7 +5240,7 @@
       </c>
       <c r="R18" s="6"/>
     </row>
-    <row r="19" spans="1:18" ht="87" hidden="1">
+    <row r="19" spans="1:18" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
         <v>32</v>
       </c>
@@ -5274,7 +5292,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="87" hidden="1">
+    <row r="20" spans="1:18" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
         <v>32</v>
       </c>
@@ -5322,7 +5340,7 @@
       <c r="Q20" s="6"/>
       <c r="R20" s="6"/>
     </row>
-    <row r="21" spans="1:18" ht="116" hidden="1">
+    <row r="21" spans="1:18" ht="116" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
         <v>32</v>
       </c>
@@ -5374,7 +5392,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="174" hidden="1">
+    <row r="22" spans="1:18" ht="174" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
         <v>32</v>
       </c>
@@ -5426,7 +5444,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="116" hidden="1">
+    <row r="23" spans="1:18" ht="116" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
         <v>32</v>
       </c>
@@ -5480,7 +5498,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="72.5" hidden="1">
+    <row r="24" spans="1:18" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
         <v>32</v>
       </c>
@@ -5534,7 +5552,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="58" hidden="1">
+    <row r="25" spans="1:18" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
         <v>32</v>
       </c>
@@ -5584,7 +5602,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="159.5" hidden="1">
+    <row r="26" spans="1:18" ht="159.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
         <v>32</v>
       </c>
@@ -5638,7 +5656,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="101.5" hidden="1">
+    <row r="27" spans="1:18" ht="101.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="6" t="s">
         <v>32</v>
       </c>
@@ -5692,7 +5710,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="116" hidden="1">
+    <row r="28" spans="1:18" ht="116" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
         <v>32</v>
       </c>
@@ -5744,7 +5762,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="58" hidden="1">
+    <row r="29" spans="1:18" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="6" t="s">
         <v>32</v>
       </c>
@@ -5794,7 +5812,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="87" hidden="1">
+    <row r="30" spans="1:18" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="6" t="s">
         <v>32</v>
       </c>
@@ -5844,7 +5862,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="72.5" hidden="1">
+    <row r="31" spans="1:18" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
         <v>32</v>
       </c>
@@ -5894,7 +5912,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="72.5" hidden="1">
+    <row r="32" spans="1:18" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="6" t="s">
         <v>32</v>
       </c>
@@ -5944,7 +5962,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="101.5" hidden="1">
+    <row r="33" spans="1:18" ht="101.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="6" t="s">
         <v>32</v>
       </c>
@@ -5996,7 +6014,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="159.5" hidden="1">
+    <row r="34" spans="1:18" ht="159.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="6" t="s">
         <v>32</v>
       </c>
@@ -6048,7 +6066,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="35" spans="1:18" ht="130.5" hidden="1">
+    <row r="35" spans="1:18" ht="130.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="6" t="s">
         <v>32</v>
       </c>
@@ -6102,7 +6120,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="36" spans="1:18" ht="130.5" hidden="1">
+    <row r="36" spans="1:18" ht="130.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="6" t="s">
         <v>32</v>
       </c>
@@ -6156,7 +6174,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="217.5" hidden="1">
+    <row r="37" spans="1:18" ht="217.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="6" t="s">
         <v>32</v>
       </c>
@@ -6208,7 +6226,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="101.5" hidden="1">
+    <row r="38" spans="1:18" ht="101.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="6" t="s">
         <v>32</v>
       </c>
@@ -6258,7 +6276,7 @@
       </c>
       <c r="R38" s="6"/>
     </row>
-    <row r="39" spans="1:18" ht="145" hidden="1">
+    <row r="39" spans="1:18" ht="145" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="6" t="s">
         <v>32</v>
       </c>
@@ -6310,7 +6328,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="40" spans="1:18" ht="116" hidden="1">
+    <row r="40" spans="1:18" ht="116" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" s="6" t="s">
         <v>32</v>
       </c>
@@ -6362,7 +6380,7 @@
       </c>
       <c r="R40" s="6"/>
     </row>
-    <row r="41" spans="1:18" ht="246.5" hidden="1">
+    <row r="41" spans="1:18" ht="246.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="6" t="s">
         <v>32</v>
       </c>
@@ -6416,7 +6434,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="249.5" hidden="1" customHeight="1">
+    <row r="42" spans="1:18" ht="249.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="6" t="s">
         <v>32</v>
       </c>
@@ -6466,7 +6484,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="58" hidden="1">
+    <row r="43" spans="1:18" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" s="6" t="s">
         <v>32</v>
       </c>
@@ -6516,7 +6534,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="275.5" hidden="1" customHeight="1">
+    <row r="44" spans="1:18" ht="275.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="6" t="s">
         <v>32</v>
       </c>
@@ -6564,7 +6582,7 @@
       </c>
       <c r="R44" s="6"/>
     </row>
-    <row r="45" spans="1:18" ht="116" hidden="1">
+    <row r="45" spans="1:18" ht="116" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="6" t="s">
         <v>32</v>
       </c>
@@ -6616,7 +6634,7 @@
       </c>
       <c r="R45" s="6"/>
     </row>
-    <row r="46" spans="1:18" ht="87" hidden="1">
+    <row r="46" spans="1:18" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="6" t="s">
         <v>32</v>
       </c>
@@ -6670,7 +6688,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="47" spans="1:18" ht="116" hidden="1">
+    <row r="47" spans="1:18" ht="116" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="6" t="s">
         <v>32</v>
       </c>
@@ -6722,7 +6740,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="48" spans="1:18" ht="72.5" hidden="1">
+    <row r="48" spans="1:18" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="6" t="s">
         <v>32</v>
       </c>
@@ -6776,7 +6794,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="49" spans="1:18" ht="145" hidden="1">
+    <row r="49" spans="1:18" ht="145" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="6" t="s">
         <v>32</v>
       </c>
@@ -6830,7 +6848,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="50" spans="1:18" ht="188.5" hidden="1">
+    <row r="50" spans="1:18" ht="188.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" s="6" t="s">
         <v>32</v>
       </c>
@@ -6882,7 +6900,7 @@
       </c>
       <c r="R50" s="6"/>
     </row>
-    <row r="51" spans="1:18" ht="101.5" hidden="1">
+    <row r="51" spans="1:18" ht="101.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="6" t="s">
         <v>32</v>
       </c>
@@ -6934,7 +6952,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="52" spans="1:18" ht="58" hidden="1">
+    <row r="52" spans="1:18" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="6" t="s">
         <v>32</v>
       </c>
@@ -6986,7 +7004,7 @@
       </c>
       <c r="R52" s="6"/>
     </row>
-    <row r="53" spans="1:18" ht="188.5" hidden="1">
+    <row r="53" spans="1:18" ht="188.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="6" t="s">
         <v>32</v>
       </c>
@@ -7040,7 +7058,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="54" spans="1:18" ht="87" hidden="1">
+    <row r="54" spans="1:18" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" s="6" t="s">
         <v>32</v>
       </c>
@@ -7092,7 +7110,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="55" spans="1:18" ht="116" hidden="1">
+    <row r="55" spans="1:18" ht="116" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="6" t="s">
         <v>32</v>
       </c>
@@ -7144,7 +7162,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="56" spans="1:18" ht="116" hidden="1">
+    <row r="56" spans="1:18" ht="116" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" s="6" t="s">
         <v>32</v>
       </c>
@@ -7198,7 +7216,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="57" spans="1:18" ht="101.5" hidden="1">
+    <row r="57" spans="1:18" ht="101.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="6" t="s">
         <v>32</v>
       </c>
@@ -7252,7 +7270,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="58" spans="1:18" ht="159.5" hidden="1">
+    <row r="58" spans="1:18" ht="159.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" s="6" t="s">
         <v>32</v>
       </c>
@@ -7306,7 +7324,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="59" spans="1:18" ht="116">
+    <row r="59" spans="1:18" ht="116" x14ac:dyDescent="0.35">
       <c r="A59" s="6" t="s">
         <v>32</v>
       </c>
@@ -7356,7 +7374,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="60" spans="1:18" ht="72.5" hidden="1">
+    <row r="60" spans="1:18" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" s="6" t="s">
         <v>32</v>
       </c>
@@ -7396,7 +7414,7 @@
       <c r="Q60" s="6"/>
       <c r="R60" s="6"/>
     </row>
-    <row r="61" spans="1:18" ht="72.5">
+    <row r="61" spans="1:18" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A61" s="6" t="s">
         <v>32</v>
       </c>
@@ -7446,7 +7464,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="62" spans="1:18" ht="87">
+    <row r="62" spans="1:18" ht="87" x14ac:dyDescent="0.35">
       <c r="A62" s="6" t="s">
         <v>32</v>
       </c>
@@ -7498,7 +7516,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="63" spans="1:18" ht="304.5">
+    <row r="63" spans="1:18" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A63" s="6" t="s">
         <v>32</v>
       </c>
@@ -7548,7 +7566,7 @@
       </c>
       <c r="R63" s="6"/>
     </row>
-    <row r="64" spans="1:18" ht="101.5">
+    <row r="64" spans="1:18" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A64" s="6" t="s">
         <v>32</v>
       </c>
@@ -7598,7 +7616,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="65" spans="1:18" ht="87">
+    <row r="65" spans="1:18" ht="87" x14ac:dyDescent="0.35">
       <c r="A65" s="6" t="s">
         <v>32</v>
       </c>
@@ -7648,7 +7666,7 @@
       </c>
       <c r="R65" s="6"/>
     </row>
-    <row r="66" spans="1:18" ht="130.5">
+    <row r="66" spans="1:18" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A66" s="6" t="s">
         <v>32</v>
       </c>
@@ -7700,7 +7718,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="67" spans="1:18" ht="130.5">
+    <row r="67" spans="1:18" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A67" s="6" t="s">
         <v>32</v>
       </c>
@@ -7754,7 +7772,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="68" spans="1:18" ht="130.5">
+    <row r="68" spans="1:18" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A68" s="6" t="s">
         <v>32</v>
       </c>
@@ -7808,7 +7826,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="69" spans="1:18" ht="145">
+    <row r="69" spans="1:18" ht="145" x14ac:dyDescent="0.35">
       <c r="A69" s="6" t="s">
         <v>32</v>
       </c>
@@ -7862,7 +7880,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="70" spans="1:18" ht="87">
+    <row r="70" spans="1:18" ht="87" x14ac:dyDescent="0.35">
       <c r="A70" s="6" t="s">
         <v>32</v>
       </c>
@@ -7916,7 +7934,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="71" spans="1:18" ht="130.5">
+    <row r="71" spans="1:18" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A71" s="6" t="s">
         <v>32</v>
       </c>
@@ -7970,7 +7988,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="72" spans="1:18" ht="101.5">
+    <row r="72" spans="1:18" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A72" s="6" t="s">
         <v>32</v>
       </c>
@@ -8024,7 +8042,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="73" spans="1:18" ht="116">
+    <row r="73" spans="1:18" ht="116" x14ac:dyDescent="0.35">
       <c r="A73" s="6" t="s">
         <v>32</v>
       </c>
@@ -8078,7 +8096,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="74" spans="1:18" ht="72.5">
+    <row r="74" spans="1:18" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A74" s="6" t="s">
         <v>32</v>
       </c>
@@ -8130,7 +8148,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="75" spans="1:18" ht="72.5" hidden="1">
+    <row r="75" spans="1:18" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" s="6" t="s">
         <v>32</v>
       </c>
@@ -8178,7 +8196,7 @@
       <c r="Q75" s="6"/>
       <c r="R75" s="6"/>
     </row>
-    <row r="76" spans="1:18" ht="130.5" hidden="1">
+    <row r="76" spans="1:18" ht="130.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" s="6" t="s">
         <v>32</v>
       </c>
@@ -8228,7 +8246,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="77" spans="1:18" ht="58" hidden="1">
+    <row r="77" spans="1:18" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" s="6" t="s">
         <v>32</v>
       </c>
@@ -8280,7 +8298,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="78" spans="1:18" ht="174" hidden="1">
+    <row r="78" spans="1:18" ht="174" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" s="6" t="s">
         <v>32</v>
       </c>
@@ -8328,7 +8346,7 @@
       </c>
       <c r="R78" s="6"/>
     </row>
-    <row r="79" spans="1:18" ht="116" hidden="1">
+    <row r="79" spans="1:18" ht="116" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" s="6" t="s">
         <v>32</v>
       </c>
@@ -8380,7 +8398,7 @@
       </c>
       <c r="R79" s="6"/>
     </row>
-    <row r="80" spans="1:18" ht="145" hidden="1">
+    <row r="80" spans="1:18" ht="145" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" s="6" t="s">
         <v>32</v>
       </c>
@@ -8434,7 +8452,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="81" spans="1:18" ht="188.5" hidden="1">
+    <row r="81" spans="1:18" ht="188.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" s="6" t="s">
         <v>32</v>
       </c>
@@ -8486,7 +8504,7 @@
       </c>
       <c r="R81" s="6"/>
     </row>
-    <row r="82" spans="1:18" ht="72.5" hidden="1">
+    <row r="82" spans="1:18" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" s="6" t="s">
         <v>32</v>
       </c>
@@ -8536,7 +8554,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="83" spans="1:18" ht="304.5" hidden="1">
+    <row r="83" spans="1:18" ht="304.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" s="6" t="s">
         <v>32</v>
       </c>
@@ -8586,7 +8604,7 @@
       </c>
       <c r="R83" s="6"/>
     </row>
-    <row r="84" spans="1:18" ht="87" hidden="1">
+    <row r="84" spans="1:18" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" s="6" t="s">
         <v>32</v>
       </c>
@@ -8640,7 +8658,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="85" spans="1:18" ht="87" hidden="1">
+    <row r="85" spans="1:18" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" s="6" t="s">
         <v>32</v>
       </c>
@@ -8690,7 +8708,7 @@
       </c>
       <c r="R85" s="6"/>
     </row>
-    <row r="86" spans="1:18" ht="87" hidden="1">
+    <row r="86" spans="1:18" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" s="6" t="s">
         <v>32</v>
       </c>
@@ -8742,7 +8760,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="87" spans="1:18" ht="130.5" hidden="1">
+    <row r="87" spans="1:18" ht="130.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" s="6" t="s">
         <v>32</v>
       </c>
@@ -8796,7 +8814,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="88" spans="1:18" ht="188.5" hidden="1">
+    <row r="88" spans="1:18" ht="188.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" s="6" t="s">
         <v>32</v>
       </c>
@@ -8848,7 +8866,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="89" spans="1:18" ht="87" hidden="1">
+    <row r="89" spans="1:18" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" s="6" t="s">
         <v>32</v>
       </c>
@@ -8902,7 +8920,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="90" spans="1:18" ht="116" hidden="1">
+    <row r="90" spans="1:18" ht="116" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" s="6" t="s">
         <v>32</v>
       </c>
@@ -8954,7 +8972,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="91" spans="1:18" ht="101.5" hidden="1">
+    <row r="91" spans="1:18" ht="101.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" s="6" t="s">
         <v>32</v>
       </c>
@@ -9004,7 +9022,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="92" spans="1:18" ht="72.5">
+    <row r="92" spans="1:18" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A92" s="6" t="s">
         <v>32</v>
       </c>
@@ -9048,7 +9066,7 @@
       <c r="Q92" s="6"/>
       <c r="R92" s="6"/>
     </row>
-    <row r="93" spans="1:18" ht="101.5" hidden="1">
+    <row r="93" spans="1:18" ht="101.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" s="6" t="s">
         <v>32</v>
       </c>
@@ -9098,7 +9116,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="94" spans="1:18" ht="203" hidden="1">
+    <row r="94" spans="1:18" ht="203" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" s="6" t="s">
         <v>32</v>
       </c>
@@ -9152,7 +9170,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="95" spans="1:18" ht="116" hidden="1">
+    <row r="95" spans="1:18" ht="116" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" s="6" t="s">
         <v>32</v>
       </c>
@@ -9204,7 +9222,7 @@
       </c>
       <c r="R95" s="6"/>
     </row>
-    <row r="96" spans="1:18" ht="87" hidden="1">
+    <row r="96" spans="1:18" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" s="6" t="s">
         <v>32</v>
       </c>
@@ -9256,7 +9274,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="97" spans="1:18" ht="174" hidden="1">
+    <row r="97" spans="1:18" ht="174" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" s="6" t="s">
         <v>32</v>
       </c>
@@ -9310,7 +9328,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="98" spans="1:18" ht="72.5" hidden="1">
+    <row r="98" spans="1:18" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" s="6" t="s">
         <v>32</v>
       </c>
@@ -9362,7 +9380,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="99" spans="1:18" ht="58" hidden="1">
+    <row r="99" spans="1:18" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" s="6" t="s">
         <v>32</v>
       </c>
@@ -9412,7 +9430,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="100" spans="1:18" ht="87" hidden="1">
+    <row r="100" spans="1:18" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" s="6" t="s">
         <v>32</v>
       </c>
@@ -9466,7 +9484,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="101" spans="1:18" ht="72.5" hidden="1">
+    <row r="101" spans="1:18" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" s="6" t="s">
         <v>32</v>
       </c>
@@ -9516,7 +9534,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="102" spans="1:18" ht="130.5" hidden="1">
+    <row r="102" spans="1:18" ht="130.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" s="6" t="s">
         <v>32</v>
       </c>
@@ -9568,7 +9586,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="103" spans="1:18" ht="87" hidden="1">
+    <row r="103" spans="1:18" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" s="6" t="s">
         <v>32</v>
       </c>
@@ -9620,7 +9638,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="104" spans="1:18" ht="159.5" hidden="1">
+    <row r="104" spans="1:18" ht="159.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" s="6" t="s">
         <v>32</v>
       </c>
@@ -9670,7 +9688,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="105" spans="1:18" ht="116" hidden="1">
+    <row r="105" spans="1:18" ht="116" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105" s="6" t="s">
         <v>32</v>
       </c>
@@ -9722,7 +9740,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="106" spans="1:18" ht="101.5" hidden="1">
+    <row r="106" spans="1:18" ht="101.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106" s="6" t="s">
         <v>32</v>
       </c>
@@ -9774,7 +9792,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="107" spans="1:18" ht="72.5" hidden="1">
+    <row r="107" spans="1:18" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" s="6" t="s">
         <v>32</v>
       </c>
@@ -9826,7 +9844,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="108" spans="1:18" ht="145" hidden="1">
+    <row r="108" spans="1:18" ht="145" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" s="6" t="s">
         <v>32</v>
       </c>
@@ -9878,7 +9896,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="109" spans="1:18" ht="188.5" hidden="1">
+    <row r="109" spans="1:18" ht="188.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109" s="6" t="s">
         <v>32</v>
       </c>
@@ -9930,7 +9948,7 @@
       </c>
       <c r="R109" s="6"/>
     </row>
-    <row r="110" spans="1:18" ht="116" hidden="1">
+    <row r="110" spans="1:18" ht="116" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" s="6" t="s">
         <v>32</v>
       </c>
@@ -9982,7 +10000,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="111" spans="1:18" ht="174" hidden="1">
+    <row r="111" spans="1:18" ht="174" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" s="6" t="s">
         <v>32</v>
       </c>
@@ -10034,7 +10052,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="112" spans="1:18" ht="116" hidden="1">
+    <row r="112" spans="1:18" ht="116" hidden="1" x14ac:dyDescent="0.35">
       <c r="A112" s="6" t="s">
         <v>32</v>
       </c>
@@ -10088,7 +10106,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="113" spans="1:18" ht="145" hidden="1">
+    <row r="113" spans="1:18" ht="145" hidden="1" x14ac:dyDescent="0.35">
       <c r="A113" s="6" t="s">
         <v>32</v>
       </c>
@@ -10142,7 +10160,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="114" spans="1:18" ht="145" hidden="1">
+    <row r="114" spans="1:18" ht="145" hidden="1" x14ac:dyDescent="0.35">
       <c r="A114" s="6" t="s">
         <v>32</v>
       </c>
@@ -10192,7 +10210,7 @@
       <c r="Q114" s="6"/>
       <c r="R114" s="6"/>
     </row>
-    <row r="115" spans="1:18" ht="116" hidden="1">
+    <row r="115" spans="1:18" ht="116" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115" s="6" t="s">
         <v>32</v>
       </c>
@@ -10244,7 +10262,7 @@
       </c>
       <c r="R115" s="6"/>
     </row>
-    <row r="116" spans="1:18" ht="145" hidden="1">
+    <row r="116" spans="1:18" ht="145" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" s="6" t="s">
         <v>32</v>
       </c>
@@ -10296,7 +10314,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="117" spans="1:18" ht="188.5" hidden="1">
+    <row r="117" spans="1:18" ht="188.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117" s="6" t="s">
         <v>32</v>
       </c>
@@ -10350,7 +10368,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="118" spans="1:18" ht="130.5" hidden="1">
+    <row r="118" spans="1:18" ht="130.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A118" s="6" t="s">
         <v>32</v>
       </c>
@@ -10404,7 +10422,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="119" spans="1:18" ht="116" hidden="1">
+    <row r="119" spans="1:18" ht="116" hidden="1" x14ac:dyDescent="0.35">
       <c r="A119" s="6" t="s">
         <v>32</v>
       </c>
@@ -10456,7 +10474,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="120" spans="1:18" ht="159.5" hidden="1">
+    <row r="120" spans="1:18" ht="159.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A120" s="6" t="s">
         <v>32</v>
       </c>
@@ -10510,7 +10528,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="121" spans="1:18" ht="72.5" hidden="1">
+    <row r="121" spans="1:18" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121" s="6" t="s">
         <v>32</v>
       </c>
@@ -10556,7 +10574,7 @@
       <c r="Q121" s="6"/>
       <c r="R121" s="6"/>
     </row>
-    <row r="122" spans="1:18" ht="58" hidden="1">
+    <row r="122" spans="1:18" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A122" s="6" t="s">
         <v>32</v>
       </c>
@@ -10608,7 +10626,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="123" spans="1:18" ht="145" hidden="1">
+    <row r="123" spans="1:18" ht="145" hidden="1" x14ac:dyDescent="0.35">
       <c r="A123" s="6" t="s">
         <v>32</v>
       </c>
@@ -10662,7 +10680,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="124" spans="1:18" ht="29" hidden="1">
+    <row r="124" spans="1:18" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124" s="6" t="s">
         <v>32</v>
       </c>
@@ -10712,7 +10730,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="125" spans="1:18" ht="87" hidden="1">
+    <row r="125" spans="1:18" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125" s="6" t="s">
         <v>32</v>
       </c>
@@ -10758,7 +10776,7 @@
       <c r="Q125" s="6"/>
       <c r="R125" s="6"/>
     </row>
-    <row r="126" spans="1:18" ht="101.5" hidden="1">
+    <row r="126" spans="1:18" ht="101.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A126" s="6" t="s">
         <v>32</v>
       </c>
@@ -10808,7 +10826,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="127" spans="1:18" ht="58" hidden="1">
+    <row r="127" spans="1:18" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" s="6" t="s">
         <v>32</v>
       </c>
@@ -10860,7 +10878,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="128" spans="1:18" ht="58" hidden="1">
+    <row r="128" spans="1:18" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A128" s="6" t="s">
         <v>32</v>
       </c>
@@ -10912,7 +10930,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="129" spans="1:18" ht="72.5">
+    <row r="129" spans="1:18" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A129" s="6" t="s">
         <v>32</v>
       </c>
@@ -10954,7 +10972,7 @@
       <c r="Q129" s="6"/>
       <c r="R129" s="6"/>
     </row>
-    <row r="130" spans="1:18" ht="87" hidden="1">
+    <row r="130" spans="1:18" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="A130" s="6" t="s">
         <v>32</v>
       </c>
@@ -11004,7 +11022,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="131" spans="1:18" ht="58" hidden="1">
+    <row r="131" spans="1:18" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A131" s="6" t="s">
         <v>32</v>
       </c>
@@ -11056,7 +11074,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="132" spans="1:18" ht="145" hidden="1">
+    <row r="132" spans="1:18" ht="145" hidden="1" x14ac:dyDescent="0.35">
       <c r="A132" s="6" t="s">
         <v>32</v>
       </c>
@@ -11108,7 +11126,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="133" spans="1:18" ht="87" hidden="1">
+    <row r="133" spans="1:18" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="A133" s="6" t="s">
         <v>32</v>
       </c>
@@ -11160,7 +11178,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="134" spans="1:18" ht="188.5" hidden="1">
+    <row r="134" spans="1:18" ht="188.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A134" s="6" t="s">
         <v>32</v>
       </c>
@@ -11212,7 +11230,7 @@
       </c>
       <c r="R134" s="6"/>
     </row>
-    <row r="135" spans="1:18" ht="72.5" hidden="1">
+    <row r="135" spans="1:18" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A135" s="6" t="s">
         <v>32</v>
       </c>
@@ -11264,7 +11282,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="136" spans="1:18" ht="174" hidden="1">
+    <row r="136" spans="1:18" ht="174" hidden="1" x14ac:dyDescent="0.35">
       <c r="A136" s="6" t="s">
         <v>32</v>
       </c>
@@ -11314,7 +11332,7 @@
       </c>
       <c r="R136" s="6"/>
     </row>
-    <row r="137" spans="1:18" ht="58" hidden="1">
+    <row r="137" spans="1:18" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A137" s="6" t="s">
         <v>32</v>
       </c>
@@ -11362,7 +11380,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="138" spans="1:18" ht="72.5" hidden="1">
+    <row r="138" spans="1:18" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A138" s="6" t="s">
         <v>32</v>
       </c>
@@ -11414,7 +11432,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="139" spans="1:18" ht="43.5" hidden="1">
+    <row r="139" spans="1:18" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A139" s="6" t="s">
         <v>32</v>
       </c>
@@ -11462,7 +11480,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="140" spans="1:18" ht="72.5" hidden="1">
+    <row r="140" spans="1:18" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A140" s="6" t="s">
         <v>32</v>
       </c>
@@ -11502,7 +11520,7 @@
       <c r="Q140" s="6"/>
       <c r="R140" s="6"/>
     </row>
-    <row r="141" spans="1:18" ht="145" hidden="1">
+    <row r="141" spans="1:18" ht="145" hidden="1" x14ac:dyDescent="0.35">
       <c r="A141" s="6" t="s">
         <v>32</v>
       </c>
@@ -11552,7 +11570,7 @@
       </c>
       <c r="R141" s="6"/>
     </row>
-    <row r="142" spans="1:18" ht="58" hidden="1">
+    <row r="142" spans="1:18" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A142" s="6" t="s">
         <v>32</v>
       </c>
@@ -11602,7 +11620,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="143" spans="1:18" ht="130.5" hidden="1">
+    <row r="143" spans="1:18" ht="130.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A143" s="6" t="s">
         <v>32</v>
       </c>
@@ -11654,7 +11672,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="144" spans="1:18" ht="87" hidden="1">
+    <row r="144" spans="1:18" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="A144" s="6" t="s">
         <v>32</v>
       </c>
@@ -11706,7 +11724,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="145" spans="1:18" ht="58" hidden="1">
+    <row r="145" spans="1:18" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A145" s="6" t="s">
         <v>32</v>
       </c>
@@ -11756,7 +11774,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="146" spans="1:18" ht="130.5" hidden="1">
+    <row r="146" spans="1:18" ht="130.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A146" s="6" t="s">
         <v>32</v>
       </c>
@@ -11808,7 +11826,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="147" spans="1:18" ht="58" hidden="1">
+    <row r="147" spans="1:18" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A147" s="6" t="s">
         <v>32</v>
       </c>
@@ -11856,7 +11874,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="148" spans="1:18" ht="116" hidden="1">
+    <row r="148" spans="1:18" ht="116" hidden="1" x14ac:dyDescent="0.35">
       <c r="A148" s="6" t="s">
         <v>32</v>
       </c>
@@ -11910,7 +11928,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="149" spans="1:18" ht="72.5" hidden="1">
+    <row r="149" spans="1:18" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A149" s="6" t="s">
         <v>32</v>
       </c>
@@ -11958,7 +11976,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="150" spans="1:18" ht="87" hidden="1">
+    <row r="150" spans="1:18" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="A150" s="6" t="s">
         <v>32</v>
       </c>
@@ -12010,7 +12028,7 @@
       </c>
       <c r="R150" s="6"/>
     </row>
-    <row r="151" spans="1:18" ht="87" hidden="1">
+    <row r="151" spans="1:18" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="A151" s="6" t="s">
         <v>32</v>
       </c>
@@ -12062,7 +12080,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="152" spans="1:18" ht="72.5" hidden="1">
+    <row r="152" spans="1:18" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A152" s="6" t="s">
         <v>32</v>
       </c>
@@ -12112,7 +12130,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="153" spans="1:18" ht="72.5" hidden="1">
+    <row r="153" spans="1:18" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A153" s="6" t="s">
         <v>32</v>
       </c>
@@ -12162,7 +12180,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="154" spans="1:18" ht="72.5" hidden="1">
+    <row r="154" spans="1:18" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A154" s="6" t="s">
         <v>32</v>
       </c>
@@ -12216,7 +12234,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="155" spans="1:18" ht="58" hidden="1">
+    <row r="155" spans="1:18" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A155" s="6" t="s">
         <v>32</v>
       </c>
@@ -12264,7 +12282,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="156" spans="1:18" ht="87" hidden="1">
+    <row r="156" spans="1:18" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="A156" s="6" t="s">
         <v>32</v>
       </c>
@@ -12316,7 +12334,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="157" spans="1:18" ht="87" hidden="1">
+    <row r="157" spans="1:18" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="A157" s="6" t="s">
         <v>32</v>
       </c>
@@ -12368,7 +12386,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="158" spans="1:18" ht="174" hidden="1">
+    <row r="158" spans="1:18" ht="174" hidden="1" x14ac:dyDescent="0.35">
       <c r="A158" s="6" t="s">
         <v>32</v>
       </c>
@@ -12420,7 +12438,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="159" spans="1:18" ht="116" hidden="1">
+    <row r="159" spans="1:18" ht="116" hidden="1" x14ac:dyDescent="0.35">
       <c r="A159" s="6" t="s">
         <v>32</v>
       </c>
@@ -12470,7 +12488,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="160" spans="1:18" ht="101.5" hidden="1">
+    <row r="160" spans="1:18" ht="101.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A160" s="6" t="s">
         <v>32</v>
       </c>
@@ -12522,7 +12540,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="161" spans="1:18" ht="145" hidden="1">
+    <row r="161" spans="1:18" ht="145" hidden="1" x14ac:dyDescent="0.35">
       <c r="A161" s="6" t="s">
         <v>32</v>
       </c>
@@ -12576,7 +12594,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="162" spans="1:18" ht="159.5" hidden="1">
+    <row r="162" spans="1:18" ht="159.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A162" s="6" t="s">
         <v>32</v>
       </c>
@@ -12628,7 +12646,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="163" spans="1:18" ht="188.5" hidden="1">
+    <row r="163" spans="1:18" ht="188.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A163" s="6" t="s">
         <v>32</v>
       </c>
@@ -12680,7 +12698,7 @@
       </c>
       <c r="R163" s="6"/>
     </row>
-    <row r="164" spans="1:18" ht="130.5" hidden="1">
+    <row r="164" spans="1:18" ht="130.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A164" s="6" t="s">
         <v>32</v>
       </c>
@@ -12734,7 +12752,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="165" spans="1:18" ht="29" hidden="1">
+    <row r="165" spans="1:18" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A165" s="6" t="s">
         <v>32</v>
       </c>
@@ -12772,7 +12790,7 @@
       <c r="Q165" s="6"/>
       <c r="R165" s="6"/>
     </row>
-    <row r="166" spans="1:18" ht="116" hidden="1">
+    <row r="166" spans="1:18" ht="116" hidden="1" x14ac:dyDescent="0.35">
       <c r="A166" s="6" t="s">
         <v>32</v>
       </c>
@@ -12822,7 +12840,7 @@
       </c>
       <c r="R166" s="6"/>
     </row>
-    <row r="167" spans="1:18" ht="145" hidden="1">
+    <row r="167" spans="1:18" ht="145" hidden="1" x14ac:dyDescent="0.35">
       <c r="A167" s="6" t="s">
         <v>32</v>
       </c>
@@ -12874,7 +12892,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="168" spans="1:18" ht="43.5" hidden="1">
+    <row r="168" spans="1:18" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A168" s="6" t="s">
         <v>32</v>
       </c>
@@ -12912,7 +12930,7 @@
       <c r="Q168" s="6"/>
       <c r="R168" s="6"/>
     </row>
-    <row r="169" spans="1:18" ht="116" hidden="1">
+    <row r="169" spans="1:18" ht="116" hidden="1" x14ac:dyDescent="0.35">
       <c r="A169" s="6" t="s">
         <v>32</v>
       </c>
@@ -12966,7 +12984,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="170" spans="1:18" ht="101.5" hidden="1">
+    <row r="170" spans="1:18" ht="101.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A170" s="6" t="s">
         <v>32</v>
       </c>
@@ -13020,7 +13038,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="171" spans="1:18" ht="87" hidden="1">
+    <row r="171" spans="1:18" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="A171" s="6" t="s">
         <v>32</v>
       </c>
@@ -13072,7 +13090,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="172" spans="1:18" ht="87" hidden="1">
+    <row r="172" spans="1:18" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="A172" s="6" t="s">
         <v>32</v>
       </c>
@@ -13126,7 +13144,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="173" spans="1:18" ht="72.5" hidden="1">
+    <row r="173" spans="1:18" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A173" s="6" t="s">
         <v>32</v>
       </c>
@@ -13176,7 +13194,7 @@
       </c>
       <c r="R173" s="6"/>
     </row>
-    <row r="174" spans="1:18" ht="87" hidden="1">
+    <row r="174" spans="1:18" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="A174" s="6" t="s">
         <v>32</v>
       </c>
@@ -13230,7 +13248,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="175" spans="1:18" ht="72.5" hidden="1">
+    <row r="175" spans="1:18" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A175" s="6" t="s">
         <v>32</v>
       </c>
@@ -13272,7 +13290,7 @@
       <c r="Q175" s="6"/>
       <c r="R175" s="6"/>
     </row>
-    <row r="176" spans="1:18" ht="130.5" hidden="1">
+    <row r="176" spans="1:18" ht="130.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A176" s="6" t="s">
         <v>32</v>
       </c>
@@ -13314,7 +13332,7 @@
       <c r="Q176" s="6"/>
       <c r="R176" s="6"/>
     </row>
-    <row r="177" spans="1:18" ht="159.5" hidden="1">
+    <row r="177" spans="1:18" ht="159.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A177" s="6" t="s">
         <v>32</v>
       </c>
@@ -13356,7 +13374,7 @@
       <c r="Q177" s="6"/>
       <c r="R177" s="6"/>
     </row>
-    <row r="178" spans="1:18" ht="72.5" hidden="1">
+    <row r="178" spans="1:18" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A178" s="6" t="s">
         <v>32</v>
       </c>
@@ -13398,7 +13416,7 @@
       <c r="Q178" s="6"/>
       <c r="R178" s="6"/>
     </row>
-    <row r="179" spans="1:18" ht="43.5" hidden="1">
+    <row r="179" spans="1:18" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A179" s="6" t="s">
         <v>32</v>
       </c>
@@ -13440,7 +13458,7 @@
       <c r="Q179" s="6"/>
       <c r="R179" s="6"/>
     </row>
-    <row r="180" spans="1:18" ht="58" hidden="1">
+    <row r="180" spans="1:18" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A180" s="6" t="s">
         <v>32</v>
       </c>
@@ -13482,7 +13500,7 @@
       <c r="Q180" s="6"/>
       <c r="R180" s="6"/>
     </row>
-    <row r="181" spans="1:18" ht="72.5" hidden="1">
+    <row r="181" spans="1:18" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A181" s="6" t="s">
         <v>32</v>
       </c>
@@ -13524,7 +13542,7 @@
       <c r="Q181" s="6"/>
       <c r="R181" s="6"/>
     </row>
-    <row r="182" spans="1:18" ht="58" hidden="1">
+    <row r="182" spans="1:18" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A182" s="6" t="s">
         <v>32</v>
       </c>
@@ -13566,7 +13584,7 @@
       <c r="Q182" s="6"/>
       <c r="R182" s="6"/>
     </row>
-    <row r="183" spans="1:18" ht="116" hidden="1">
+    <row r="183" spans="1:18" ht="116" hidden="1" x14ac:dyDescent="0.35">
       <c r="A183" s="6" t="s">
         <v>32</v>
       </c>
@@ -13608,7 +13626,7 @@
       <c r="Q183" s="6"/>
       <c r="R183" s="6"/>
     </row>
-    <row r="184" spans="1:18" ht="87" hidden="1">
+    <row r="184" spans="1:18" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="A184" s="6" t="s">
         <v>32</v>
       </c>
@@ -13650,7 +13668,7 @@
       <c r="Q184" s="6"/>
       <c r="R184" s="6"/>
     </row>
-    <row r="185" spans="1:18" ht="58" hidden="1">
+    <row r="185" spans="1:18" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A185" s="6" t="s">
         <v>32</v>
       </c>
@@ -13692,7 +13710,7 @@
       <c r="Q185" s="6"/>
       <c r="R185" s="6"/>
     </row>
-    <row r="186" spans="1:18" ht="87" hidden="1">
+    <row r="186" spans="1:18" ht="87" hidden="1" x14ac:dyDescent="0.35">
       <c r="A186" s="6" t="s">
         <v>32</v>
       </c>
@@ -13736,7 +13754,7 @@
       <c r="Q186" s="6"/>
       <c r="R186" s="6"/>
     </row>
-    <row r="187" spans="1:18">
+    <row r="187" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A187" s="6" t="s">
         <v>32</v>
       </c>
@@ -13761,6 +13779,58 @@
       <c r="P187" s="6"/>
       <c r="Q187" s="6"/>
       <c r="R187" s="6"/>
+    </row>
+    <row r="188" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A188" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B188" s="6" t="s">
+        <v>400</v>
+      </c>
+      <c r="C188" s="6" t="s">
+        <v>1104</v>
+      </c>
+      <c r="D188" s="6" t="s">
+        <v>1102</v>
+      </c>
+      <c r="I188" s="6"/>
+      <c r="L188" s="6"/>
+      <c r="M188" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="N188" s="6" t="s">
+        <v>1106</v>
+      </c>
+      <c r="O188" s="6"/>
+      <c r="P188" s="6"/>
+      <c r="Q188" s="6"/>
+      <c r="R188" s="6"/>
+    </row>
+    <row r="189" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A189" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B189" s="6" t="s">
+        <v>400</v>
+      </c>
+      <c r="C189" s="6" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D189" s="6" t="s">
+        <v>1102</v>
+      </c>
+      <c r="I189" s="6"/>
+      <c r="L189" s="6"/>
+      <c r="M189" s="6" t="s">
+        <v>1108</v>
+      </c>
+      <c r="N189" s="6" t="s">
+        <v>1109</v>
+      </c>
+      <c r="O189" s="6"/>
+      <c r="P189" s="6"/>
+      <c r="Q189" s="6"/>
+      <c r="R189" s="6"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:R186" xr:uid="{00000000-0009-0000-0000-000001000000}">

</xml_diff>

<commit_message>
ajout lecture du fichier excel au hal mining
</commit_message>
<xml_diff>
--- a/Data/FairCarboN_RNSR_copie.xlsx
+++ b/Data/FairCarboN_RNSR_copie.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dutroncj\Documents\Outils\FairCarboN_datas\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F656DC-C8E0-4FEF-B8B9-60BE5975648A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DFE8C83-F885-4C80-98BE-82D62E6CBD7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
     <sheet name="Liste" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Liste!$A$1:$Q$376</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Liste!$A$1:$Q$378</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4102" uniqueCount="1600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4114" uniqueCount="1603">
   <si>
     <t>Titre : Liste des unités du PEPR FairCarboN</t>
   </si>
@@ -5223,12 +5223,21 @@
   <si>
     <t>6.1749763</t>
   </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Jérôme Demarty</t>
+  </si>
+  <si>
+    <t>Jean-Philippe Jenny</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5730,51 +5739,51 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="13.6328125" customWidth="1"/>
     <col min="3" max="3" width="19.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="43.5">
+    <row r="10" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
@@ -5782,7 +5791,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="58">
+    <row r="12" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="B12" s="7" t="s">
         <v>9</v>
       </c>
@@ -5790,7 +5799,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="29">
+    <row r="13" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="B13" s="8" t="s">
         <v>11</v>
       </c>
@@ -5798,7 +5807,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="43.5">
+    <row r="14" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B14" s="9" t="s">
         <v>13</v>
       </c>
@@ -5806,7 +5815,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -5819,16 +5828,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:Q376"/>
+  <dimension ref="A1:Q378"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A167" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A348" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="R4" sqref="R4"/>
-      <selection pane="bottomLeft" activeCell="T382" sqref="T382"/>
+      <selection pane="bottomLeft" activeCell="J380" sqref="J380"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.54296875" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.453125" style="10" bestFit="1" customWidth="1"/>
@@ -5850,7 +5858,7 @@
     <col min="18" max="16384" width="8.7265625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="11" customFormat="1">
+    <row r="1" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>16</v>
       </c>
@@ -5903,7 +5911,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="72.5">
+    <row r="2" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>32</v>
       </c>
@@ -5956,7 +5964,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="58">
+    <row r="3" spans="1:17" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>32</v>
       </c>
@@ -6005,7 +6013,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="174">
+    <row r="4" spans="1:17" ht="174" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>32</v>
       </c>
@@ -6054,7 +6062,7 @@
       </c>
       <c r="Q4" s="6"/>
     </row>
-    <row r="5" spans="1:17" ht="87">
+    <row r="5" spans="1:17" ht="87" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>32</v>
       </c>
@@ -6107,7 +6115,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="145">
+    <row r="6" spans="1:17" ht="145" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>32</v>
       </c>
@@ -6156,7 +6164,7 @@
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
     </row>
-    <row r="7" spans="1:17" ht="116">
+    <row r="7" spans="1:17" ht="116" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>32</v>
       </c>
@@ -6207,7 +6215,7 @@
       </c>
       <c r="Q7" s="6"/>
     </row>
-    <row r="8" spans="1:17" ht="159.5">
+    <row r="8" spans="1:17" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>32</v>
       </c>
@@ -6260,7 +6268,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="87">
+    <row r="9" spans="1:17" ht="87" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>32</v>
       </c>
@@ -6313,7 +6321,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="116">
+    <row r="10" spans="1:17" ht="116" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>32</v>
       </c>
@@ -6364,7 +6372,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="72.5">
+    <row r="11" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>32</v>
       </c>
@@ -6417,7 +6425,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="101.5">
+    <row r="12" spans="1:17" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>32</v>
       </c>
@@ -6466,7 +6474,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="188.5">
+    <row r="13" spans="1:17" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>32</v>
       </c>
@@ -6517,7 +6525,7 @@
       </c>
       <c r="Q13" s="6"/>
     </row>
-    <row r="14" spans="1:17" ht="174">
+    <row r="14" spans="1:17" ht="174" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>32</v>
       </c>
@@ -6568,7 +6576,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="101.5">
+    <row r="15" spans="1:17" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>32</v>
       </c>
@@ -6615,7 +6623,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="87">
+    <row r="16" spans="1:17" ht="87" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>32</v>
       </c>
@@ -6666,7 +6674,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="101.5">
+    <row r="17" spans="1:17" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
         <v>32</v>
       </c>
@@ -6717,7 +6725,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="58">
+    <row r="18" spans="1:17" ht="58" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
         <v>32</v>
       </c>
@@ -6768,7 +6776,7 @@
       </c>
       <c r="Q18" s="6"/>
     </row>
-    <row r="19" spans="1:17" ht="87">
+    <row r="19" spans="1:17" ht="87" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
         <v>32</v>
       </c>
@@ -6819,7 +6827,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="87">
+    <row r="20" spans="1:17" ht="87" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
         <v>32</v>
       </c>
@@ -6866,7 +6874,7 @@
       <c r="P20" s="6"/>
       <c r="Q20" s="6"/>
     </row>
-    <row r="21" spans="1:17" ht="116">
+    <row r="21" spans="1:17" ht="116" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
         <v>32</v>
       </c>
@@ -6917,7 +6925,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="174">
+    <row r="22" spans="1:17" ht="174" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
         <v>32</v>
       </c>
@@ -6968,7 +6976,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="116">
+    <row r="23" spans="1:17" ht="116" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
         <v>32</v>
       </c>
@@ -7021,7 +7029,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="72.5">
+    <row r="24" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
         <v>32</v>
       </c>
@@ -7074,7 +7082,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="58">
+    <row r="25" spans="1:17" ht="58" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
         <v>32</v>
       </c>
@@ -7123,7 +7131,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="159.5">
+    <row r="26" spans="1:17" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
         <v>32</v>
       </c>
@@ -7176,7 +7184,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="101.5">
+    <row r="27" spans="1:17" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A27" s="6" t="s">
         <v>32</v>
       </c>
@@ -7229,7 +7237,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="116">
+    <row r="28" spans="1:17" ht="116" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
         <v>32</v>
       </c>
@@ -7280,7 +7288,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="58">
+    <row r="29" spans="1:17" ht="58" x14ac:dyDescent="0.35">
       <c r="A29" s="6" t="s">
         <v>32</v>
       </c>
@@ -7329,7 +7337,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="87">
+    <row r="30" spans="1:17" ht="87" x14ac:dyDescent="0.35">
       <c r="A30" s="6" t="s">
         <v>32</v>
       </c>
@@ -7378,7 +7386,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="72.5">
+    <row r="31" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
         <v>32</v>
       </c>
@@ -7427,7 +7435,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="72.5">
+    <row r="32" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A32" s="6" t="s">
         <v>32</v>
       </c>
@@ -7476,7 +7484,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="101.5">
+    <row r="33" spans="1:17" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A33" s="6" t="s">
         <v>32</v>
       </c>
@@ -7527,7 +7535,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="159.5">
+    <row r="34" spans="1:17" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A34" s="6" t="s">
         <v>32</v>
       </c>
@@ -7578,7 +7586,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="130.5">
+    <row r="35" spans="1:17" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A35" s="6" t="s">
         <v>32</v>
       </c>
@@ -7631,7 +7639,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="130.5">
+    <row r="36" spans="1:17" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A36" s="6" t="s">
         <v>32</v>
       </c>
@@ -7684,7 +7692,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="217.5">
+    <row r="37" spans="1:17" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A37" s="6" t="s">
         <v>32</v>
       </c>
@@ -7735,7 +7743,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="101.5">
+    <row r="38" spans="1:17" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A38" s="6" t="s">
         <v>32</v>
       </c>
@@ -7784,7 +7792,7 @@
       </c>
       <c r="Q38" s="6"/>
     </row>
-    <row r="39" spans="1:17" ht="145">
+    <row r="39" spans="1:17" ht="145" x14ac:dyDescent="0.35">
       <c r="A39" s="6" t="s">
         <v>32</v>
       </c>
@@ -7835,7 +7843,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="116">
+    <row r="40" spans="1:17" ht="116" x14ac:dyDescent="0.35">
       <c r="A40" s="6" t="s">
         <v>32</v>
       </c>
@@ -7886,7 +7894,7 @@
       </c>
       <c r="Q40" s="6"/>
     </row>
-    <row r="41" spans="1:17" ht="246.5">
+    <row r="41" spans="1:17" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A41" s="6" t="s">
         <v>32</v>
       </c>
@@ -7939,7 +7947,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="249.5" customHeight="1">
+    <row r="42" spans="1:17" ht="249.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="6" t="s">
         <v>32</v>
       </c>
@@ -7988,7 +7996,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="43" spans="1:17" ht="58">
+    <row r="43" spans="1:17" ht="58" x14ac:dyDescent="0.35">
       <c r="A43" s="6" t="s">
         <v>32</v>
       </c>
@@ -8037,7 +8045,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="275.5" customHeight="1">
+    <row r="44" spans="1:17" ht="275.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="6" t="s">
         <v>32</v>
       </c>
@@ -8084,7 +8092,7 @@
       </c>
       <c r="Q44" s="6"/>
     </row>
-    <row r="45" spans="1:17" ht="116">
+    <row r="45" spans="1:17" ht="116" x14ac:dyDescent="0.35">
       <c r="A45" s="6" t="s">
         <v>32</v>
       </c>
@@ -8135,7 +8143,7 @@
       </c>
       <c r="Q45" s="6"/>
     </row>
-    <row r="46" spans="1:17" ht="87">
+    <row r="46" spans="1:17" ht="87" x14ac:dyDescent="0.35">
       <c r="A46" s="6" t="s">
         <v>32</v>
       </c>
@@ -8188,7 +8196,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="47" spans="1:17" ht="116">
+    <row r="47" spans="1:17" ht="116" x14ac:dyDescent="0.35">
       <c r="A47" s="6" t="s">
         <v>32</v>
       </c>
@@ -8239,7 +8247,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="48" spans="1:17" ht="72.5">
+    <row r="48" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A48" s="6" t="s">
         <v>32</v>
       </c>
@@ -8292,7 +8300,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="49" spans="1:17" ht="145">
+    <row r="49" spans="1:17" ht="145" x14ac:dyDescent="0.35">
       <c r="A49" s="6" t="s">
         <v>32</v>
       </c>
@@ -8345,7 +8353,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="50" spans="1:17" ht="188.5">
+    <row r="50" spans="1:17" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A50" s="6" t="s">
         <v>32</v>
       </c>
@@ -8396,7 +8404,7 @@
       </c>
       <c r="Q50" s="6"/>
     </row>
-    <row r="51" spans="1:17" ht="101.5">
+    <row r="51" spans="1:17" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A51" s="6" t="s">
         <v>32</v>
       </c>
@@ -8447,7 +8455,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="52" spans="1:17" ht="58">
+    <row r="52" spans="1:17" ht="58" x14ac:dyDescent="0.35">
       <c r="A52" s="6" t="s">
         <v>32</v>
       </c>
@@ -8498,7 +8506,7 @@
       </c>
       <c r="Q52" s="6"/>
     </row>
-    <row r="53" spans="1:17" ht="188.5">
+    <row r="53" spans="1:17" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A53" s="6" t="s">
         <v>32</v>
       </c>
@@ -8551,7 +8559,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="54" spans="1:17" ht="87">
+    <row r="54" spans="1:17" ht="87" x14ac:dyDescent="0.35">
       <c r="A54" s="6" t="s">
         <v>32</v>
       </c>
@@ -8602,7 +8610,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="55" spans="1:17" ht="116">
+    <row r="55" spans="1:17" ht="116" x14ac:dyDescent="0.35">
       <c r="A55" s="6" t="s">
         <v>32</v>
       </c>
@@ -8653,7 +8661,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="56" spans="1:17" ht="116">
+    <row r="56" spans="1:17" ht="116" x14ac:dyDescent="0.35">
       <c r="A56" s="6" t="s">
         <v>32</v>
       </c>
@@ -8706,7 +8714,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="57" spans="1:17" ht="101.5">
+    <row r="57" spans="1:17" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A57" s="6" t="s">
         <v>32</v>
       </c>
@@ -8759,7 +8767,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="58" spans="1:17" ht="159.5">
+    <row r="58" spans="1:17" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A58" s="6" t="s">
         <v>32</v>
       </c>
@@ -8812,7 +8820,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="59" spans="1:17" ht="116">
+    <row r="59" spans="1:17" ht="116" x14ac:dyDescent="0.35">
       <c r="A59" s="6" t="s">
         <v>32</v>
       </c>
@@ -8861,7 +8869,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="60" spans="1:17" ht="72.5">
+    <row r="60" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A60" s="6" t="s">
         <v>32</v>
       </c>
@@ -8900,7 +8908,7 @@
       <c r="P60" s="6"/>
       <c r="Q60" s="6"/>
     </row>
-    <row r="61" spans="1:17" ht="72.5">
+    <row r="61" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A61" s="6" t="s">
         <v>32</v>
       </c>
@@ -8949,7 +8957,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="62" spans="1:17" ht="87">
+    <row r="62" spans="1:17" ht="87" x14ac:dyDescent="0.35">
       <c r="A62" s="6" t="s">
         <v>32</v>
       </c>
@@ -9000,7 +9008,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="63" spans="1:17" ht="304.5">
+    <row r="63" spans="1:17" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A63" s="6" t="s">
         <v>32</v>
       </c>
@@ -9049,7 +9057,7 @@
       </c>
       <c r="Q63" s="6"/>
     </row>
-    <row r="64" spans="1:17" ht="101.5">
+    <row r="64" spans="1:17" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A64" s="6" t="s">
         <v>32</v>
       </c>
@@ -9098,7 +9106,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="65" spans="1:17" ht="87">
+    <row r="65" spans="1:17" ht="87" x14ac:dyDescent="0.35">
       <c r="A65" s="6" t="s">
         <v>32</v>
       </c>
@@ -9147,7 +9155,7 @@
       </c>
       <c r="Q65" s="6"/>
     </row>
-    <row r="66" spans="1:17" ht="130.5">
+    <row r="66" spans="1:17" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A66" s="6" t="s">
         <v>32</v>
       </c>
@@ -9198,7 +9206,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="67" spans="1:17" ht="130.5">
+    <row r="67" spans="1:17" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A67" s="6" t="s">
         <v>32</v>
       </c>
@@ -9251,7 +9259,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="68" spans="1:17" ht="130.5">
+    <row r="68" spans="1:17" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A68" s="6" t="s">
         <v>32</v>
       </c>
@@ -9304,7 +9312,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="69" spans="1:17" ht="145">
+    <row r="69" spans="1:17" ht="145" x14ac:dyDescent="0.35">
       <c r="A69" s="6" t="s">
         <v>32</v>
       </c>
@@ -9357,7 +9365,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="70" spans="1:17" ht="87">
+    <row r="70" spans="1:17" ht="87" x14ac:dyDescent="0.35">
       <c r="A70" s="6" t="s">
         <v>32</v>
       </c>
@@ -9410,7 +9418,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="71" spans="1:17" ht="130.5">
+    <row r="71" spans="1:17" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A71" s="6" t="s">
         <v>32</v>
       </c>
@@ -9463,7 +9471,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="72" spans="1:17" ht="101.5">
+    <row r="72" spans="1:17" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A72" s="6" t="s">
         <v>32</v>
       </c>
@@ -9516,7 +9524,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="73" spans="1:17" ht="116">
+    <row r="73" spans="1:17" ht="116" x14ac:dyDescent="0.35">
       <c r="A73" s="6" t="s">
         <v>32</v>
       </c>
@@ -9569,7 +9577,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="74" spans="1:17" ht="72.5">
+    <row r="74" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A74" s="6" t="s">
         <v>32</v>
       </c>
@@ -9620,7 +9628,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="75" spans="1:17" ht="72.5">
+    <row r="75" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A75" s="6" t="s">
         <v>32</v>
       </c>
@@ -9667,7 +9675,7 @@
       <c r="P75" s="6"/>
       <c r="Q75" s="6"/>
     </row>
-    <row r="76" spans="1:17" ht="130.5">
+    <row r="76" spans="1:17" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A76" s="6" t="s">
         <v>32</v>
       </c>
@@ -9716,7 +9724,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="77" spans="1:17" ht="58">
+    <row r="77" spans="1:17" ht="58" x14ac:dyDescent="0.35">
       <c r="A77" s="6" t="s">
         <v>32</v>
       </c>
@@ -9767,7 +9775,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="78" spans="1:17" ht="174">
+    <row r="78" spans="1:17" ht="174" x14ac:dyDescent="0.35">
       <c r="A78" s="6" t="s">
         <v>32</v>
       </c>
@@ -9814,7 +9822,7 @@
       </c>
       <c r="Q78" s="6"/>
     </row>
-    <row r="79" spans="1:17" ht="116">
+    <row r="79" spans="1:17" ht="116" x14ac:dyDescent="0.35">
       <c r="A79" s="6" t="s">
         <v>32</v>
       </c>
@@ -9865,7 +9873,7 @@
       </c>
       <c r="Q79" s="6"/>
     </row>
-    <row r="80" spans="1:17" ht="145">
+    <row r="80" spans="1:17" ht="145" x14ac:dyDescent="0.35">
       <c r="A80" s="6" t="s">
         <v>32</v>
       </c>
@@ -9918,7 +9926,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="81" spans="1:17" ht="188.5">
+    <row r="81" spans="1:17" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A81" s="6" t="s">
         <v>32</v>
       </c>
@@ -9969,7 +9977,7 @@
       </c>
       <c r="Q81" s="6"/>
     </row>
-    <row r="82" spans="1:17" ht="72.5">
+    <row r="82" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A82" s="6" t="s">
         <v>32</v>
       </c>
@@ -10018,7 +10026,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="83" spans="1:17" ht="304.5">
+    <row r="83" spans="1:17" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A83" s="6" t="s">
         <v>32</v>
       </c>
@@ -10067,7 +10075,7 @@
       </c>
       <c r="Q83" s="6"/>
     </row>
-    <row r="84" spans="1:17" ht="87">
+    <row r="84" spans="1:17" ht="87" x14ac:dyDescent="0.35">
       <c r="A84" s="6" t="s">
         <v>32</v>
       </c>
@@ -10120,7 +10128,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="85" spans="1:17" ht="87">
+    <row r="85" spans="1:17" ht="87" x14ac:dyDescent="0.35">
       <c r="A85" s="6" t="s">
         <v>32</v>
       </c>
@@ -10169,7 +10177,7 @@
       </c>
       <c r="Q85" s="6"/>
     </row>
-    <row r="86" spans="1:17" ht="87">
+    <row r="86" spans="1:17" ht="87" x14ac:dyDescent="0.35">
       <c r="A86" s="6" t="s">
         <v>32</v>
       </c>
@@ -10220,7 +10228,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="87" spans="1:17" ht="130.5">
+    <row r="87" spans="1:17" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A87" s="6" t="s">
         <v>32</v>
       </c>
@@ -10273,7 +10281,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="88" spans="1:17" ht="188.5">
+    <row r="88" spans="1:17" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A88" s="6" t="s">
         <v>32</v>
       </c>
@@ -10324,7 +10332,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="89" spans="1:17" ht="87">
+    <row r="89" spans="1:17" ht="87" x14ac:dyDescent="0.35">
       <c r="A89" s="6" t="s">
         <v>32</v>
       </c>
@@ -10377,7 +10385,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="90" spans="1:17" ht="116">
+    <row r="90" spans="1:17" ht="116" x14ac:dyDescent="0.35">
       <c r="A90" s="6" t="s">
         <v>32</v>
       </c>
@@ -10428,7 +10436,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="91" spans="1:17" ht="101.5">
+    <row r="91" spans="1:17" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A91" s="6" t="s">
         <v>32</v>
       </c>
@@ -10477,7 +10485,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="92" spans="1:17" ht="72.5">
+    <row r="92" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A92" s="6" t="s">
         <v>32</v>
       </c>
@@ -10520,7 +10528,7 @@
       <c r="P92" s="6"/>
       <c r="Q92" s="6"/>
     </row>
-    <row r="93" spans="1:17" ht="101.5">
+    <row r="93" spans="1:17" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A93" s="6" t="s">
         <v>32</v>
       </c>
@@ -10569,7 +10577,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="94" spans="1:17" ht="203">
+    <row r="94" spans="1:17" ht="203" x14ac:dyDescent="0.35">
       <c r="A94" s="6" t="s">
         <v>32</v>
       </c>
@@ -10622,7 +10630,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="95" spans="1:17" ht="116">
+    <row r="95" spans="1:17" ht="116" x14ac:dyDescent="0.35">
       <c r="A95" s="6" t="s">
         <v>32</v>
       </c>
@@ -10673,7 +10681,7 @@
       </c>
       <c r="Q95" s="6"/>
     </row>
-    <row r="96" spans="1:17" ht="87">
+    <row r="96" spans="1:17" ht="87" x14ac:dyDescent="0.35">
       <c r="A96" s="6" t="s">
         <v>32</v>
       </c>
@@ -10724,7 +10732,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="97" spans="1:17" ht="174">
+    <row r="97" spans="1:17" ht="174" x14ac:dyDescent="0.35">
       <c r="A97" s="6" t="s">
         <v>32</v>
       </c>
@@ -10777,7 +10785,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="98" spans="1:17" ht="72.5">
+    <row r="98" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A98" s="6" t="s">
         <v>32</v>
       </c>
@@ -10828,7 +10836,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="99" spans="1:17" ht="58">
+    <row r="99" spans="1:17" ht="58" x14ac:dyDescent="0.35">
       <c r="A99" s="6" t="s">
         <v>32</v>
       </c>
@@ -10877,7 +10885,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="100" spans="1:17" ht="87">
+    <row r="100" spans="1:17" ht="87" x14ac:dyDescent="0.35">
       <c r="A100" s="6" t="s">
         <v>32</v>
       </c>
@@ -10930,7 +10938,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="101" spans="1:17" ht="72.5">
+    <row r="101" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A101" s="6" t="s">
         <v>32</v>
       </c>
@@ -10979,7 +10987,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="102" spans="1:17" ht="130.5">
+    <row r="102" spans="1:17" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A102" s="6" t="s">
         <v>32</v>
       </c>
@@ -11030,7 +11038,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="103" spans="1:17" ht="87">
+    <row r="103" spans="1:17" ht="87" x14ac:dyDescent="0.35">
       <c r="A103" s="6" t="s">
         <v>32</v>
       </c>
@@ -11081,7 +11089,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="104" spans="1:17" ht="159.5">
+    <row r="104" spans="1:17" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A104" s="6" t="s">
         <v>32</v>
       </c>
@@ -11130,7 +11138,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="105" spans="1:17" ht="116">
+    <row r="105" spans="1:17" ht="116" x14ac:dyDescent="0.35">
       <c r="A105" s="6" t="s">
         <v>32</v>
       </c>
@@ -11181,7 +11189,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="106" spans="1:17" ht="101.5">
+    <row r="106" spans="1:17" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A106" s="6" t="s">
         <v>32</v>
       </c>
@@ -11232,7 +11240,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="107" spans="1:17" ht="72.5">
+    <row r="107" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A107" s="6" t="s">
         <v>32</v>
       </c>
@@ -11283,7 +11291,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="108" spans="1:17" ht="145">
+    <row r="108" spans="1:17" ht="145" x14ac:dyDescent="0.35">
       <c r="A108" s="6" t="s">
         <v>32</v>
       </c>
@@ -11334,7 +11342,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="109" spans="1:17" ht="188.5">
+    <row r="109" spans="1:17" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A109" s="6" t="s">
         <v>32</v>
       </c>
@@ -11385,7 +11393,7 @@
       </c>
       <c r="Q109" s="6"/>
     </row>
-    <row r="110" spans="1:17" ht="116">
+    <row r="110" spans="1:17" ht="116" x14ac:dyDescent="0.35">
       <c r="A110" s="6" t="s">
         <v>32</v>
       </c>
@@ -11436,7 +11444,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="111" spans="1:17" ht="174">
+    <row r="111" spans="1:17" ht="174" x14ac:dyDescent="0.35">
       <c r="A111" s="6" t="s">
         <v>32</v>
       </c>
@@ -11487,7 +11495,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="112" spans="1:17" ht="116">
+    <row r="112" spans="1:17" ht="116" x14ac:dyDescent="0.35">
       <c r="A112" s="6" t="s">
         <v>32</v>
       </c>
@@ -11540,7 +11548,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="113" spans="1:17" ht="145">
+    <row r="113" spans="1:17" ht="145" x14ac:dyDescent="0.35">
       <c r="A113" s="6" t="s">
         <v>32</v>
       </c>
@@ -11593,7 +11601,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="114" spans="1:17" ht="145">
+    <row r="114" spans="1:17" ht="145" x14ac:dyDescent="0.35">
       <c r="A114" s="6" t="s">
         <v>32</v>
       </c>
@@ -11642,7 +11650,7 @@
       <c r="P114" s="6"/>
       <c r="Q114" s="6"/>
     </row>
-    <row r="115" spans="1:17" ht="116">
+    <row r="115" spans="1:17" ht="116" x14ac:dyDescent="0.35">
       <c r="A115" s="6" t="s">
         <v>32</v>
       </c>
@@ -11693,7 +11701,7 @@
       </c>
       <c r="Q115" s="6"/>
     </row>
-    <row r="116" spans="1:17" ht="145">
+    <row r="116" spans="1:17" ht="145" x14ac:dyDescent="0.35">
       <c r="A116" s="6" t="s">
         <v>32</v>
       </c>
@@ -11744,7 +11752,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="117" spans="1:17" ht="188.5">
+    <row r="117" spans="1:17" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A117" s="6" t="s">
         <v>32</v>
       </c>
@@ -11797,7 +11805,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="118" spans="1:17" ht="130.5">
+    <row r="118" spans="1:17" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A118" s="6" t="s">
         <v>32</v>
       </c>
@@ -11850,7 +11858,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="119" spans="1:17" ht="116">
+    <row r="119" spans="1:17" ht="116" x14ac:dyDescent="0.35">
       <c r="A119" s="6" t="s">
         <v>32</v>
       </c>
@@ -11901,7 +11909,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="120" spans="1:17" ht="159.5">
+    <row r="120" spans="1:17" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A120" s="6" t="s">
         <v>32</v>
       </c>
@@ -11954,7 +11962,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="121" spans="1:17" ht="72.5">
+    <row r="121" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A121" s="6" t="s">
         <v>32</v>
       </c>
@@ -11999,7 +12007,7 @@
       <c r="P121" s="6"/>
       <c r="Q121" s="6"/>
     </row>
-    <row r="122" spans="1:17" ht="58">
+    <row r="122" spans="1:17" ht="58" x14ac:dyDescent="0.35">
       <c r="A122" s="6" t="s">
         <v>32</v>
       </c>
@@ -12050,7 +12058,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="123" spans="1:17" ht="145">
+    <row r="123" spans="1:17" ht="145" x14ac:dyDescent="0.35">
       <c r="A123" s="6" t="s">
         <v>32</v>
       </c>
@@ -12103,7 +12111,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="124" spans="1:17" ht="29">
+    <row r="124" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A124" s="6" t="s">
         <v>32</v>
       </c>
@@ -12152,7 +12160,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="125" spans="1:17" ht="87">
+    <row r="125" spans="1:17" ht="87" x14ac:dyDescent="0.35">
       <c r="A125" s="6" t="s">
         <v>32</v>
       </c>
@@ -12197,7 +12205,7 @@
       <c r="P125" s="6"/>
       <c r="Q125" s="6"/>
     </row>
-    <row r="126" spans="1:17" ht="101.5">
+    <row r="126" spans="1:17" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A126" s="6" t="s">
         <v>32</v>
       </c>
@@ -12246,7 +12254,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="127" spans="1:17" ht="58">
+    <row r="127" spans="1:17" ht="58" x14ac:dyDescent="0.35">
       <c r="A127" s="6" t="s">
         <v>32</v>
       </c>
@@ -12297,7 +12305,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="128" spans="1:17" ht="72.5">
+    <row r="128" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A128" s="6" t="s">
         <v>32</v>
       </c>
@@ -12338,7 +12346,7 @@
       <c r="P128" s="6"/>
       <c r="Q128" s="6"/>
     </row>
-    <row r="129" spans="1:17" ht="87">
+    <row r="129" spans="1:17" ht="87" x14ac:dyDescent="0.35">
       <c r="A129" s="6" t="s">
         <v>32</v>
       </c>
@@ -12387,7 +12395,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="130" spans="1:17" ht="58">
+    <row r="130" spans="1:17" ht="58" x14ac:dyDescent="0.35">
       <c r="A130" s="6" t="s">
         <v>32</v>
       </c>
@@ -12438,7 +12446,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="131" spans="1:17" ht="145">
+    <row r="131" spans="1:17" ht="145" x14ac:dyDescent="0.35">
       <c r="A131" s="6" t="s">
         <v>32</v>
       </c>
@@ -12489,7 +12497,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="132" spans="1:17" ht="87">
+    <row r="132" spans="1:17" ht="87" x14ac:dyDescent="0.35">
       <c r="A132" s="6" t="s">
         <v>32</v>
       </c>
@@ -12540,7 +12548,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="133" spans="1:17" ht="188.5">
+    <row r="133" spans="1:17" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A133" s="6" t="s">
         <v>32</v>
       </c>
@@ -12591,7 +12599,7 @@
       </c>
       <c r="Q133" s="6"/>
     </row>
-    <row r="134" spans="1:17" ht="72.5">
+    <row r="134" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A134" s="6" t="s">
         <v>32</v>
       </c>
@@ -12642,7 +12650,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="135" spans="1:17" ht="174">
+    <row r="135" spans="1:17" ht="174" x14ac:dyDescent="0.35">
       <c r="A135" s="6" t="s">
         <v>32</v>
       </c>
@@ -12691,7 +12699,7 @@
       </c>
       <c r="Q135" s="6"/>
     </row>
-    <row r="136" spans="1:17" ht="58">
+    <row r="136" spans="1:17" ht="58" x14ac:dyDescent="0.35">
       <c r="A136" s="6" t="s">
         <v>32</v>
       </c>
@@ -12738,7 +12746,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="137" spans="1:17" ht="72.5">
+    <row r="137" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A137" s="6" t="s">
         <v>32</v>
       </c>
@@ -12789,7 +12797,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="138" spans="1:17" ht="43.5">
+    <row r="138" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A138" s="6" t="s">
         <v>32</v>
       </c>
@@ -12836,7 +12844,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="139" spans="1:17" ht="72.5">
+    <row r="139" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A139" s="6" t="s">
         <v>32</v>
       </c>
@@ -12875,7 +12883,7 @@
       <c r="P139" s="6"/>
       <c r="Q139" s="6"/>
     </row>
-    <row r="140" spans="1:17" ht="145">
+    <row r="140" spans="1:17" ht="145" x14ac:dyDescent="0.35">
       <c r="A140" s="6" t="s">
         <v>32</v>
       </c>
@@ -12924,7 +12932,7 @@
       </c>
       <c r="Q140" s="6"/>
     </row>
-    <row r="141" spans="1:17" ht="58">
+    <row r="141" spans="1:17" ht="58" x14ac:dyDescent="0.35">
       <c r="A141" s="6" t="s">
         <v>32</v>
       </c>
@@ -12973,7 +12981,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="142" spans="1:17" ht="130.5">
+    <row r="142" spans="1:17" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A142" s="6" t="s">
         <v>32</v>
       </c>
@@ -13024,7 +13032,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="143" spans="1:17" ht="87">
+    <row r="143" spans="1:17" ht="87" x14ac:dyDescent="0.35">
       <c r="A143" s="6" t="s">
         <v>32</v>
       </c>
@@ -13075,7 +13083,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="144" spans="1:17" ht="58">
+    <row r="144" spans="1:17" ht="58" x14ac:dyDescent="0.35">
       <c r="A144" s="6" t="s">
         <v>32</v>
       </c>
@@ -13124,7 +13132,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="145" spans="1:17" ht="130.5">
+    <row r="145" spans="1:17" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A145" s="6" t="s">
         <v>32</v>
       </c>
@@ -13175,7 +13183,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="146" spans="1:17" ht="72.5">
+    <row r="146" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A146" s="6" t="s">
         <v>32</v>
       </c>
@@ -13224,7 +13232,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="147" spans="1:17" ht="116">
+    <row r="147" spans="1:17" ht="116" x14ac:dyDescent="0.35">
       <c r="A147" s="6" t="s">
         <v>32</v>
       </c>
@@ -13277,7 +13285,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="148" spans="1:17" ht="72.5">
+    <row r="148" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A148" s="6" t="s">
         <v>32</v>
       </c>
@@ -13324,7 +13332,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="149" spans="1:17" ht="87">
+    <row r="149" spans="1:17" ht="87" x14ac:dyDescent="0.35">
       <c r="A149" s="6" t="s">
         <v>32</v>
       </c>
@@ -13375,7 +13383,7 @@
       </c>
       <c r="Q149" s="6"/>
     </row>
-    <row r="150" spans="1:17" ht="87">
+    <row r="150" spans="1:17" ht="87" x14ac:dyDescent="0.35">
       <c r="A150" s="6" t="s">
         <v>32</v>
       </c>
@@ -13426,7 +13434,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="151" spans="1:17" ht="72.5">
+    <row r="151" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A151" s="6" t="s">
         <v>32</v>
       </c>
@@ -13475,7 +13483,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="152" spans="1:17" ht="72.5">
+    <row r="152" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A152" s="6" t="s">
         <v>32</v>
       </c>
@@ -13524,7 +13532,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="153" spans="1:17" ht="72.5">
+    <row r="153" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A153" s="6" t="s">
         <v>32</v>
       </c>
@@ -13577,7 +13585,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="154" spans="1:17" ht="58">
+    <row r="154" spans="1:17" ht="58" x14ac:dyDescent="0.35">
       <c r="A154" s="6" t="s">
         <v>32</v>
       </c>
@@ -13624,7 +13632,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="155" spans="1:17" ht="87">
+    <row r="155" spans="1:17" ht="87" x14ac:dyDescent="0.35">
       <c r="A155" s="6" t="s">
         <v>32</v>
       </c>
@@ -13675,7 +13683,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="156" spans="1:17" ht="87">
+    <row r="156" spans="1:17" ht="87" x14ac:dyDescent="0.35">
       <c r="A156" s="6" t="s">
         <v>32</v>
       </c>
@@ -13726,7 +13734,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="157" spans="1:17" ht="174">
+    <row r="157" spans="1:17" ht="174" x14ac:dyDescent="0.35">
       <c r="A157" s="6" t="s">
         <v>32</v>
       </c>
@@ -13777,7 +13785,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="158" spans="1:17" ht="116">
+    <row r="158" spans="1:17" ht="116" x14ac:dyDescent="0.35">
       <c r="A158" s="6" t="s">
         <v>32</v>
       </c>
@@ -13826,7 +13834,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="159" spans="1:17" ht="101.5">
+    <row r="159" spans="1:17" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A159" s="6" t="s">
         <v>32</v>
       </c>
@@ -13877,7 +13885,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="160" spans="1:17" ht="145">
+    <row r="160" spans="1:17" ht="145" x14ac:dyDescent="0.35">
       <c r="A160" s="6" t="s">
         <v>32</v>
       </c>
@@ -13930,7 +13938,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="161" spans="1:17" ht="159.5">
+    <row r="161" spans="1:17" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A161" s="6" t="s">
         <v>32</v>
       </c>
@@ -13981,7 +13989,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="162" spans="1:17" ht="188.5">
+    <row r="162" spans="1:17" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A162" s="6" t="s">
         <v>32</v>
       </c>
@@ -14032,7 +14040,7 @@
       </c>
       <c r="Q162" s="6"/>
     </row>
-    <row r="163" spans="1:17" ht="130.5">
+    <row r="163" spans="1:17" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A163" s="6" t="s">
         <v>32</v>
       </c>
@@ -14085,7 +14093,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="164" spans="1:17" ht="29">
+    <row r="164" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A164" s="6" t="s">
         <v>32</v>
       </c>
@@ -14122,7 +14130,7 @@
       <c r="P164" s="6"/>
       <c r="Q164" s="6"/>
     </row>
-    <row r="165" spans="1:17" ht="116">
+    <row r="165" spans="1:17" ht="116" x14ac:dyDescent="0.35">
       <c r="A165" s="6" t="s">
         <v>32</v>
       </c>
@@ -14171,7 +14179,7 @@
       </c>
       <c r="Q165" s="6"/>
     </row>
-    <row r="166" spans="1:17" ht="145">
+    <row r="166" spans="1:17" ht="145" x14ac:dyDescent="0.35">
       <c r="A166" s="6" t="s">
         <v>32</v>
       </c>
@@ -14222,7 +14230,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="167" spans="1:17" ht="43.5">
+    <row r="167" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A167" s="6" t="s">
         <v>32</v>
       </c>
@@ -14259,7 +14267,7 @@
       <c r="P167" s="6"/>
       <c r="Q167" s="6"/>
     </row>
-    <row r="168" spans="1:17" ht="116">
+    <row r="168" spans="1:17" ht="116" x14ac:dyDescent="0.35">
       <c r="A168" s="6" t="s">
         <v>32</v>
       </c>
@@ -14312,7 +14320,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="169" spans="1:17" ht="101.5">
+    <row r="169" spans="1:17" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A169" s="6" t="s">
         <v>32</v>
       </c>
@@ -14365,7 +14373,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="170" spans="1:17" ht="87">
+    <row r="170" spans="1:17" ht="87" x14ac:dyDescent="0.35">
       <c r="A170" s="6" t="s">
         <v>32</v>
       </c>
@@ -14416,7 +14424,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="171" spans="1:17" ht="87">
+    <row r="171" spans="1:17" ht="87" x14ac:dyDescent="0.35">
       <c r="A171" s="6" t="s">
         <v>32</v>
       </c>
@@ -14469,7 +14477,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="172" spans="1:17" ht="72.5">
+    <row r="172" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A172" s="6" t="s">
         <v>32</v>
       </c>
@@ -14518,7 +14526,7 @@
       </c>
       <c r="Q172" s="6"/>
     </row>
-    <row r="173" spans="1:17" ht="87">
+    <row r="173" spans="1:17" ht="87" x14ac:dyDescent="0.35">
       <c r="A173" s="6" t="s">
         <v>32</v>
       </c>
@@ -14571,7 +14579,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="174" spans="1:17" ht="72.5">
+    <row r="174" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A174" s="6" t="s">
         <v>32</v>
       </c>
@@ -14612,7 +14620,7 @@
       <c r="P174" s="6"/>
       <c r="Q174" s="6"/>
     </row>
-    <row r="175" spans="1:17" ht="130.5">
+    <row r="175" spans="1:17" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A175" s="6" t="s">
         <v>32</v>
       </c>
@@ -14653,7 +14661,7 @@
       <c r="P175" s="6"/>
       <c r="Q175" s="6"/>
     </row>
-    <row r="176" spans="1:17" ht="159.5">
+    <row r="176" spans="1:17" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A176" s="6" t="s">
         <v>32</v>
       </c>
@@ -14694,7 +14702,7 @@
       <c r="P176" s="6"/>
       <c r="Q176" s="6"/>
     </row>
-    <row r="177" spans="1:17" ht="72.5">
+    <row r="177" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A177" s="6" t="s">
         <v>32</v>
       </c>
@@ -14735,7 +14743,7 @@
       <c r="P177" s="6"/>
       <c r="Q177" s="6"/>
     </row>
-    <row r="178" spans="1:17" ht="43.5">
+    <row r="178" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A178" s="6" t="s">
         <v>32</v>
       </c>
@@ -14776,7 +14784,7 @@
       <c r="P178" s="6"/>
       <c r="Q178" s="6"/>
     </row>
-    <row r="179" spans="1:17" ht="58">
+    <row r="179" spans="1:17" ht="58" x14ac:dyDescent="0.35">
       <c r="A179" s="6" t="s">
         <v>32</v>
       </c>
@@ -14817,7 +14825,7 @@
       <c r="P179" s="6"/>
       <c r="Q179" s="6"/>
     </row>
-    <row r="180" spans="1:17" ht="72.5">
+    <row r="180" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A180" s="6" t="s">
         <v>32</v>
       </c>
@@ -14858,7 +14866,7 @@
       <c r="P180" s="6"/>
       <c r="Q180" s="6"/>
     </row>
-    <row r="181" spans="1:17" ht="58">
+    <row r="181" spans="1:17" ht="58" x14ac:dyDescent="0.35">
       <c r="A181" s="6" t="s">
         <v>32</v>
       </c>
@@ -14899,7 +14907,7 @@
       <c r="P181" s="6"/>
       <c r="Q181" s="6"/>
     </row>
-    <row r="182" spans="1:17" ht="116">
+    <row r="182" spans="1:17" ht="116" x14ac:dyDescent="0.35">
       <c r="A182" s="6" t="s">
         <v>32</v>
       </c>
@@ -14940,7 +14948,7 @@
       <c r="P182" s="6"/>
       <c r="Q182" s="6"/>
     </row>
-    <row r="183" spans="1:17" ht="87">
+    <row r="183" spans="1:17" ht="87" x14ac:dyDescent="0.35">
       <c r="A183" s="6" t="s">
         <v>32</v>
       </c>
@@ -14981,7 +14989,7 @@
       <c r="P183" s="6"/>
       <c r="Q183" s="6"/>
     </row>
-    <row r="184" spans="1:17" ht="58">
+    <row r="184" spans="1:17" ht="58" x14ac:dyDescent="0.35">
       <c r="A184" s="6" t="s">
         <v>32</v>
       </c>
@@ -15022,7 +15030,7 @@
       <c r="P184" s="6"/>
       <c r="Q184" s="6"/>
     </row>
-    <row r="185" spans="1:17" ht="87">
+    <row r="185" spans="1:17" ht="87" x14ac:dyDescent="0.35">
       <c r="A185" s="6" t="s">
         <v>32</v>
       </c>
@@ -15065,7 +15073,7 @@
       <c r="P185" s="6"/>
       <c r="Q185" s="6"/>
     </row>
-    <row r="186" spans="1:17" hidden="1">
+    <row r="186" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A186" s="6" t="s">
         <v>32</v>
       </c>
@@ -15096,7 +15104,7 @@
       <c r="P186" s="6"/>
       <c r="Q186" s="6"/>
     </row>
-    <row r="187" spans="1:17" hidden="1">
+    <row r="187" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A187" s="6" t="s">
         <v>32</v>
       </c>
@@ -15127,7 +15135,7 @@
       <c r="P187" s="6"/>
       <c r="Q187" s="6"/>
     </row>
-    <row r="188" spans="1:17" hidden="1">
+    <row r="188" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A188" s="6" t="s">
         <v>32</v>
       </c>
@@ -15158,7 +15166,7 @@
       <c r="P188" s="6"/>
       <c r="Q188" s="6"/>
     </row>
-    <row r="189" spans="1:17" hidden="1">
+    <row r="189" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A189" s="6" t="s">
         <v>32</v>
       </c>
@@ -15189,7 +15197,7 @@
       <c r="P189" s="6"/>
       <c r="Q189" s="6"/>
     </row>
-    <row r="190" spans="1:17" hidden="1">
+    <row r="190" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A190" s="6" t="s">
         <v>32</v>
       </c>
@@ -15220,7 +15228,7 @@
       <c r="P190" s="6"/>
       <c r="Q190" s="6"/>
     </row>
-    <row r="191" spans="1:17" hidden="1">
+    <row r="191" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A191" s="6" t="s">
         <v>32</v>
       </c>
@@ -15251,7 +15259,7 @@
       <c r="P191" s="6"/>
       <c r="Q191" s="6"/>
     </row>
-    <row r="192" spans="1:17" hidden="1">
+    <row r="192" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A192" s="6" t="s">
         <v>32</v>
       </c>
@@ -15282,7 +15290,7 @@
       <c r="P192" s="6"/>
       <c r="Q192" s="6"/>
     </row>
-    <row r="193" spans="1:17" hidden="1">
+    <row r="193" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A193" s="6" t="s">
         <v>32</v>
       </c>
@@ -15313,7 +15321,7 @@
       <c r="P193" s="6"/>
       <c r="Q193" s="6"/>
     </row>
-    <row r="194" spans="1:17" hidden="1">
+    <row r="194" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A194" s="6" t="s">
         <v>32</v>
       </c>
@@ -15344,7 +15352,7 @@
       <c r="P194" s="6"/>
       <c r="Q194" s="6"/>
     </row>
-    <row r="195" spans="1:17" hidden="1">
+    <row r="195" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A195" s="6" t="s">
         <v>32</v>
       </c>
@@ -15375,7 +15383,7 @@
       <c r="P195" s="6"/>
       <c r="Q195" s="6"/>
     </row>
-    <row r="196" spans="1:17" hidden="1">
+    <row r="196" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A196" s="6" t="s">
         <v>32</v>
       </c>
@@ -15406,7 +15414,7 @@
       <c r="P196" s="6"/>
       <c r="Q196" s="6"/>
     </row>
-    <row r="197" spans="1:17" hidden="1">
+    <row r="197" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A197" s="6" t="s">
         <v>32</v>
       </c>
@@ -15437,7 +15445,7 @@
       <c r="P197" s="6"/>
       <c r="Q197" s="6"/>
     </row>
-    <row r="198" spans="1:17" hidden="1">
+    <row r="198" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A198" s="6" t="s">
         <v>32</v>
       </c>
@@ -15468,7 +15476,7 @@
       <c r="P198" s="6"/>
       <c r="Q198" s="6"/>
     </row>
-    <row r="199" spans="1:17" hidden="1">
+    <row r="199" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A199" s="6" t="s">
         <v>32</v>
       </c>
@@ -15499,7 +15507,7 @@
       <c r="P199" s="6"/>
       <c r="Q199" s="6"/>
     </row>
-    <row r="200" spans="1:17" hidden="1">
+    <row r="200" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A200" s="6" t="s">
         <v>32</v>
       </c>
@@ -15530,7 +15538,7 @@
       <c r="P200" s="6"/>
       <c r="Q200" s="6"/>
     </row>
-    <row r="201" spans="1:17" hidden="1">
+    <row r="201" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A201" s="6" t="s">
         <v>32</v>
       </c>
@@ -15561,7 +15569,7 @@
       <c r="P201" s="6"/>
       <c r="Q201" s="6"/>
     </row>
-    <row r="202" spans="1:17" hidden="1">
+    <row r="202" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A202" s="6" t="s">
         <v>32</v>
       </c>
@@ -15592,7 +15600,7 @@
       <c r="P202" s="6"/>
       <c r="Q202" s="6"/>
     </row>
-    <row r="203" spans="1:17" hidden="1">
+    <row r="203" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A203" s="6" t="s">
         <v>32</v>
       </c>
@@ -15623,7 +15631,7 @@
       <c r="P203" s="6"/>
       <c r="Q203" s="6"/>
     </row>
-    <row r="204" spans="1:17" hidden="1">
+    <row r="204" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A204" s="6" t="s">
         <v>32</v>
       </c>
@@ -15654,7 +15662,7 @@
       <c r="P204" s="6"/>
       <c r="Q204" s="6"/>
     </row>
-    <row r="205" spans="1:17" hidden="1">
+    <row r="205" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A205" s="6" t="s">
         <v>32</v>
       </c>
@@ -15685,7 +15693,7 @@
       <c r="P205" s="6"/>
       <c r="Q205" s="6"/>
     </row>
-    <row r="206" spans="1:17" hidden="1">
+    <row r="206" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A206" s="6" t="s">
         <v>32</v>
       </c>
@@ -15716,7 +15724,7 @@
       <c r="P206" s="6"/>
       <c r="Q206" s="6"/>
     </row>
-    <row r="207" spans="1:17" hidden="1">
+    <row r="207" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A207" s="6" t="s">
         <v>32</v>
       </c>
@@ -15747,7 +15755,7 @@
       <c r="P207" s="6"/>
       <c r="Q207" s="6"/>
     </row>
-    <row r="208" spans="1:17" hidden="1">
+    <row r="208" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A208" s="6" t="s">
         <v>32</v>
       </c>
@@ -15778,7 +15786,7 @@
       <c r="P208" s="6"/>
       <c r="Q208" s="6"/>
     </row>
-    <row r="209" spans="1:17" hidden="1">
+    <row r="209" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A209" s="6" t="s">
         <v>32</v>
       </c>
@@ -15809,7 +15817,7 @@
       <c r="P209" s="6"/>
       <c r="Q209" s="6"/>
     </row>
-    <row r="210" spans="1:17" hidden="1">
+    <row r="210" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A210" s="6" t="s">
         <v>32</v>
       </c>
@@ -15840,7 +15848,7 @@
       <c r="P210" s="6"/>
       <c r="Q210" s="6"/>
     </row>
-    <row r="211" spans="1:17" hidden="1">
+    <row r="211" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A211" s="6" t="s">
         <v>32</v>
       </c>
@@ -15871,7 +15879,7 @@
       <c r="P211" s="6"/>
       <c r="Q211" s="6"/>
     </row>
-    <row r="212" spans="1:17" hidden="1">
+    <row r="212" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A212" s="6" t="s">
         <v>32</v>
       </c>
@@ -15902,7 +15910,7 @@
       <c r="P212" s="6"/>
       <c r="Q212" s="6"/>
     </row>
-    <row r="213" spans="1:17" hidden="1">
+    <row r="213" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A213" s="6" t="s">
         <v>32</v>
       </c>
@@ -15933,7 +15941,7 @@
       <c r="P213" s="6"/>
       <c r="Q213" s="6"/>
     </row>
-    <row r="214" spans="1:17" hidden="1">
+    <row r="214" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A214" s="6" t="s">
         <v>32</v>
       </c>
@@ -15964,7 +15972,7 @@
       <c r="P214" s="6"/>
       <c r="Q214" s="6"/>
     </row>
-    <row r="215" spans="1:17" hidden="1">
+    <row r="215" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A215" s="6" t="s">
         <v>32</v>
       </c>
@@ -15995,7 +16003,7 @@
       <c r="P215" s="6"/>
       <c r="Q215" s="6"/>
     </row>
-    <row r="216" spans="1:17" hidden="1">
+    <row r="216" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A216" s="6" t="s">
         <v>32</v>
       </c>
@@ -16026,7 +16034,7 @@
       <c r="P216" s="6"/>
       <c r="Q216" s="6"/>
     </row>
-    <row r="217" spans="1:17" hidden="1">
+    <row r="217" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A217" s="6" t="s">
         <v>32</v>
       </c>
@@ -16057,7 +16065,7 @@
       <c r="P217" s="6"/>
       <c r="Q217" s="6"/>
     </row>
-    <row r="218" spans="1:17" hidden="1">
+    <row r="218" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A218" s="6" t="s">
         <v>32</v>
       </c>
@@ -16088,7 +16096,7 @@
       <c r="P218" s="6"/>
       <c r="Q218" s="6"/>
     </row>
-    <row r="219" spans="1:17" hidden="1">
+    <row r="219" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A219" s="6" t="s">
         <v>32</v>
       </c>
@@ -16119,7 +16127,7 @@
       <c r="P219" s="6"/>
       <c r="Q219" s="6"/>
     </row>
-    <row r="220" spans="1:17" hidden="1">
+    <row r="220" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A220" s="6" t="s">
         <v>32</v>
       </c>
@@ -16150,7 +16158,7 @@
       <c r="P220" s="6"/>
       <c r="Q220" s="6"/>
     </row>
-    <row r="221" spans="1:17" hidden="1">
+    <row r="221" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A221" s="6" t="s">
         <v>32</v>
       </c>
@@ -16181,7 +16189,7 @@
       <c r="P221" s="6"/>
       <c r="Q221" s="6"/>
     </row>
-    <row r="222" spans="1:17" hidden="1">
+    <row r="222" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A222" s="6" t="s">
         <v>32</v>
       </c>
@@ -16212,7 +16220,7 @@
       <c r="P222" s="6"/>
       <c r="Q222" s="6"/>
     </row>
-    <row r="223" spans="1:17" hidden="1">
+    <row r="223" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A223" s="6" t="s">
         <v>32</v>
       </c>
@@ -16243,7 +16251,7 @@
       <c r="P223" s="6"/>
       <c r="Q223" s="6"/>
     </row>
-    <row r="224" spans="1:17" hidden="1">
+    <row r="224" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A224" s="6" t="s">
         <v>32</v>
       </c>
@@ -16274,7 +16282,7 @@
       <c r="P224" s="6"/>
       <c r="Q224" s="6"/>
     </row>
-    <row r="225" spans="1:17" hidden="1">
+    <row r="225" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A225" s="6" t="s">
         <v>32</v>
       </c>
@@ -16305,7 +16313,7 @@
       <c r="P225" s="6"/>
       <c r="Q225" s="6"/>
     </row>
-    <row r="226" spans="1:17" hidden="1">
+    <row r="226" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A226" s="6" t="s">
         <v>32</v>
       </c>
@@ -16336,7 +16344,7 @@
       <c r="P226" s="6"/>
       <c r="Q226" s="6"/>
     </row>
-    <row r="227" spans="1:17" hidden="1">
+    <row r="227" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A227" s="6" t="s">
         <v>32</v>
       </c>
@@ -16367,7 +16375,7 @@
       <c r="P227" s="6"/>
       <c r="Q227" s="6"/>
     </row>
-    <row r="228" spans="1:17" hidden="1">
+    <row r="228" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A228" s="6" t="s">
         <v>32</v>
       </c>
@@ -16398,7 +16406,7 @@
       <c r="P228" s="6"/>
       <c r="Q228" s="6"/>
     </row>
-    <row r="229" spans="1:17" hidden="1">
+    <row r="229" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A229" s="6" t="s">
         <v>32</v>
       </c>
@@ -16429,7 +16437,7 @@
       <c r="P229" s="6"/>
       <c r="Q229" s="6"/>
     </row>
-    <row r="230" spans="1:17" hidden="1">
+    <row r="230" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A230" s="6" t="s">
         <v>32</v>
       </c>
@@ -16460,7 +16468,7 @@
       <c r="P230" s="6"/>
       <c r="Q230" s="6"/>
     </row>
-    <row r="231" spans="1:17" hidden="1">
+    <row r="231" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A231" s="6" t="s">
         <v>32</v>
       </c>
@@ -16491,7 +16499,7 @@
       <c r="P231" s="6"/>
       <c r="Q231" s="6"/>
     </row>
-    <row r="232" spans="1:17" hidden="1">
+    <row r="232" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A232" s="6" t="s">
         <v>32</v>
       </c>
@@ -16522,7 +16530,7 @@
       <c r="P232" s="6"/>
       <c r="Q232" s="6"/>
     </row>
-    <row r="233" spans="1:17" hidden="1">
+    <row r="233" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A233" s="6" t="s">
         <v>32</v>
       </c>
@@ -16553,7 +16561,7 @@
       <c r="P233" s="6"/>
       <c r="Q233" s="6"/>
     </row>
-    <row r="234" spans="1:17" hidden="1">
+    <row r="234" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A234" s="6" t="s">
         <v>32</v>
       </c>
@@ -16584,7 +16592,7 @@
       <c r="P234" s="6"/>
       <c r="Q234" s="6"/>
     </row>
-    <row r="235" spans="1:17" hidden="1">
+    <row r="235" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A235" s="6" t="s">
         <v>32</v>
       </c>
@@ -16615,7 +16623,7 @@
       <c r="P235" s="6"/>
       <c r="Q235" s="6"/>
     </row>
-    <row r="236" spans="1:17" hidden="1">
+    <row r="236" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A236" s="6" t="s">
         <v>32</v>
       </c>
@@ -16646,7 +16654,7 @@
       <c r="P236" s="6"/>
       <c r="Q236" s="6"/>
     </row>
-    <row r="237" spans="1:17" hidden="1">
+    <row r="237" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A237" s="6" t="s">
         <v>32</v>
       </c>
@@ -16677,7 +16685,7 @@
       <c r="P237" s="6"/>
       <c r="Q237" s="6"/>
     </row>
-    <row r="238" spans="1:17" s="15" customFormat="1" ht="145">
+    <row r="238" spans="1:17" s="15" customFormat="1" ht="145" x14ac:dyDescent="0.35">
       <c r="A238" s="6" t="s">
         <v>32</v>
       </c>
@@ -16730,7 +16738,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="239" spans="1:17" s="15" customFormat="1" ht="101.5">
+    <row r="239" spans="1:17" s="15" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A239" s="6" t="s">
         <v>32</v>
       </c>
@@ -16779,7 +16787,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="240" spans="1:17" s="15" customFormat="1" ht="130.5">
+    <row r="240" spans="1:17" s="15" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A240" s="6" t="s">
         <v>32</v>
       </c>
@@ -16822,7 +16830,7 @@
       <c r="P240" s="6"/>
       <c r="Q240" s="6"/>
     </row>
-    <row r="241" spans="1:17" s="15" customFormat="1" ht="116">
+    <row r="241" spans="1:17" s="15" customFormat="1" ht="116" x14ac:dyDescent="0.35">
       <c r="A241" s="6" t="s">
         <v>32</v>
       </c>
@@ -16873,7 +16881,7 @@
       </c>
       <c r="Q241" s="6"/>
     </row>
-    <row r="242" spans="1:17" s="15" customFormat="1" ht="87">
+    <row r="242" spans="1:17" s="15" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="A242" s="6" t="s">
         <v>32</v>
       </c>
@@ -16926,7 +16934,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="243" spans="1:17" s="15" customFormat="1" ht="58">
+    <row r="243" spans="1:17" s="15" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A243" s="6" t="s">
         <v>32</v>
       </c>
@@ -16969,7 +16977,7 @@
       <c r="P243" s="6"/>
       <c r="Q243" s="6"/>
     </row>
-    <row r="244" spans="1:17" ht="130.5">
+    <row r="244" spans="1:17" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A244" s="6" t="s">
         <v>32</v>
       </c>
@@ -17012,7 +17020,7 @@
       <c r="P244" s="6"/>
       <c r="Q244" s="6"/>
     </row>
-    <row r="245" spans="1:17" ht="72.5">
+    <row r="245" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A245" s="6" t="s">
         <v>32</v>
       </c>
@@ -17055,7 +17063,7 @@
       <c r="P245" s="6"/>
       <c r="Q245" s="6"/>
     </row>
-    <row r="246" spans="1:17" ht="159.5">
+    <row r="246" spans="1:17" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A246" s="6" t="s">
         <v>32</v>
       </c>
@@ -17098,7 +17106,7 @@
       <c r="P246" s="6"/>
       <c r="Q246" s="6"/>
     </row>
-    <row r="247" spans="1:17" ht="58">
+    <row r="247" spans="1:17" ht="58" x14ac:dyDescent="0.35">
       <c r="A247" s="6" t="s">
         <v>32</v>
       </c>
@@ -17137,7 +17145,7 @@
       <c r="P247" s="6"/>
       <c r="Q247" s="6"/>
     </row>
-    <row r="248" spans="1:17" ht="130.5">
+    <row r="248" spans="1:17" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A248" s="6" t="s">
         <v>32</v>
       </c>
@@ -17182,7 +17190,7 @@
       <c r="P248" s="6"/>
       <c r="Q248" s="6"/>
     </row>
-    <row r="249" spans="1:17" ht="87">
+    <row r="249" spans="1:17" ht="87" x14ac:dyDescent="0.35">
       <c r="A249" s="6" t="s">
         <v>32</v>
       </c>
@@ -17223,7 +17231,7 @@
       <c r="P249" s="6"/>
       <c r="Q249" s="6"/>
     </row>
-    <row r="250" spans="1:17" ht="72.5">
+    <row r="250" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A250" s="6" t="s">
         <v>32</v>
       </c>
@@ -17266,7 +17274,7 @@
       <c r="P250" s="6"/>
       <c r="Q250" s="6"/>
     </row>
-    <row r="251" spans="1:17" hidden="1">
+    <row r="251" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A251" s="6" t="s">
         <v>32</v>
       </c>
@@ -17297,7 +17305,7 @@
       <c r="P251" s="6"/>
       <c r="Q251" s="6"/>
     </row>
-    <row r="252" spans="1:17" hidden="1">
+    <row r="252" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A252" s="6" t="s">
         <v>32</v>
       </c>
@@ -17328,7 +17336,7 @@
       <c r="P252" s="6"/>
       <c r="Q252" s="6"/>
     </row>
-    <row r="253" spans="1:17" hidden="1">
+    <row r="253" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A253" s="6" t="s">
         <v>32</v>
       </c>
@@ -17359,7 +17367,7 @@
       <c r="P253" s="6"/>
       <c r="Q253" s="6"/>
     </row>
-    <row r="254" spans="1:17" hidden="1">
+    <row r="254" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A254" s="6" t="s">
         <v>32</v>
       </c>
@@ -17390,7 +17398,7 @@
       <c r="P254" s="6"/>
       <c r="Q254" s="6"/>
     </row>
-    <row r="255" spans="1:17" hidden="1">
+    <row r="255" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A255" s="6" t="s">
         <v>32</v>
       </c>
@@ -17421,7 +17429,7 @@
       <c r="P255" s="6"/>
       <c r="Q255" s="6"/>
     </row>
-    <row r="256" spans="1:17" hidden="1">
+    <row r="256" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A256" s="6" t="s">
         <v>32</v>
       </c>
@@ -17452,7 +17460,7 @@
       <c r="P256" s="6"/>
       <c r="Q256" s="6"/>
     </row>
-    <row r="257" spans="1:17" hidden="1">
+    <row r="257" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A257" s="6" t="s">
         <v>32</v>
       </c>
@@ -17483,7 +17491,7 @@
       <c r="P257" s="6"/>
       <c r="Q257" s="6"/>
     </row>
-    <row r="258" spans="1:17" hidden="1">
+    <row r="258" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A258" s="6" t="s">
         <v>32</v>
       </c>
@@ -17514,7 +17522,7 @@
       <c r="P258" s="6"/>
       <c r="Q258" s="6"/>
     </row>
-    <row r="259" spans="1:17" hidden="1">
+    <row r="259" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A259" s="6" t="s">
         <v>32</v>
       </c>
@@ -17545,7 +17553,7 @@
       <c r="P259" s="6"/>
       <c r="Q259" s="6"/>
     </row>
-    <row r="260" spans="1:17" hidden="1">
+    <row r="260" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A260" s="6" t="s">
         <v>32</v>
       </c>
@@ -17576,7 +17584,7 @@
       <c r="P260" s="6"/>
       <c r="Q260" s="6"/>
     </row>
-    <row r="261" spans="1:17" hidden="1">
+    <row r="261" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A261" s="6" t="s">
         <v>32</v>
       </c>
@@ -17607,7 +17615,7 @@
       <c r="P261" s="6"/>
       <c r="Q261" s="6"/>
     </row>
-    <row r="262" spans="1:17" hidden="1">
+    <row r="262" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A262" s="6" t="s">
         <v>32</v>
       </c>
@@ -17638,7 +17646,7 @@
       <c r="P262" s="6"/>
       <c r="Q262" s="6"/>
     </row>
-    <row r="263" spans="1:17" hidden="1">
+    <row r="263" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A263" s="6" t="s">
         <v>32</v>
       </c>
@@ -17669,7 +17677,7 @@
       <c r="P263" s="6"/>
       <c r="Q263" s="6"/>
     </row>
-    <row r="264" spans="1:17" hidden="1">
+    <row r="264" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A264" s="6" t="s">
         <v>32</v>
       </c>
@@ -17700,7 +17708,7 @@
       <c r="P264" s="6"/>
       <c r="Q264" s="6"/>
     </row>
-    <row r="265" spans="1:17" hidden="1">
+    <row r="265" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A265" s="6" t="s">
         <v>32</v>
       </c>
@@ -17731,7 +17739,7 @@
       <c r="P265" s="6"/>
       <c r="Q265" s="6"/>
     </row>
-    <row r="266" spans="1:17" hidden="1">
+    <row r="266" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A266" s="6" t="s">
         <v>32</v>
       </c>
@@ -17762,7 +17770,7 @@
       <c r="P266" s="6"/>
       <c r="Q266" s="6"/>
     </row>
-    <row r="267" spans="1:17" hidden="1">
+    <row r="267" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A267" s="6" t="s">
         <v>32</v>
       </c>
@@ -17793,7 +17801,7 @@
       <c r="P267" s="6"/>
       <c r="Q267" s="6"/>
     </row>
-    <row r="268" spans="1:17" hidden="1">
+    <row r="268" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A268" s="6" t="s">
         <v>32</v>
       </c>
@@ -17824,7 +17832,7 @@
       <c r="P268" s="6"/>
       <c r="Q268" s="6"/>
     </row>
-    <row r="269" spans="1:17" hidden="1">
+    <row r="269" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A269" s="6" t="s">
         <v>32</v>
       </c>
@@ -17855,7 +17863,7 @@
       <c r="P269" s="6"/>
       <c r="Q269" s="6"/>
     </row>
-    <row r="270" spans="1:17" hidden="1">
+    <row r="270" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A270" s="6" t="s">
         <v>32</v>
       </c>
@@ -17886,7 +17894,7 @@
       <c r="P270" s="6"/>
       <c r="Q270" s="6"/>
     </row>
-    <row r="271" spans="1:17" hidden="1">
+    <row r="271" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A271" s="6" t="s">
         <v>32</v>
       </c>
@@ -17917,7 +17925,7 @@
       <c r="P271" s="6"/>
       <c r="Q271" s="6"/>
     </row>
-    <row r="272" spans="1:17" hidden="1">
+    <row r="272" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A272" s="6" t="s">
         <v>32</v>
       </c>
@@ -17948,7 +17956,7 @@
       <c r="P272" s="6"/>
       <c r="Q272" s="6"/>
     </row>
-    <row r="273" spans="1:17" hidden="1">
+    <row r="273" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A273" s="6" t="s">
         <v>32</v>
       </c>
@@ -17979,7 +17987,7 @@
       <c r="P273" s="6"/>
       <c r="Q273" s="6"/>
     </row>
-    <row r="274" spans="1:17" hidden="1">
+    <row r="274" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A274" s="6" t="s">
         <v>32</v>
       </c>
@@ -18010,7 +18018,7 @@
       <c r="P274" s="6"/>
       <c r="Q274" s="6"/>
     </row>
-    <row r="275" spans="1:17" hidden="1">
+    <row r="275" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A275" s="6" t="s">
         <v>32</v>
       </c>
@@ -18041,7 +18049,7 @@
       <c r="P275" s="6"/>
       <c r="Q275" s="6"/>
     </row>
-    <row r="276" spans="1:17" hidden="1">
+    <row r="276" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A276" s="6" t="s">
         <v>32</v>
       </c>
@@ -18072,7 +18080,7 @@
       <c r="P276" s="6"/>
       <c r="Q276" s="6"/>
     </row>
-    <row r="277" spans="1:17" hidden="1">
+    <row r="277" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A277" s="6" t="s">
         <v>32</v>
       </c>
@@ -18103,7 +18111,7 @@
       <c r="P277" s="6"/>
       <c r="Q277" s="6"/>
     </row>
-    <row r="278" spans="1:17" hidden="1">
+    <row r="278" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A278" s="6" t="s">
         <v>32</v>
       </c>
@@ -18134,7 +18142,7 @@
       <c r="P278" s="6"/>
       <c r="Q278" s="6"/>
     </row>
-    <row r="279" spans="1:17" hidden="1">
+    <row r="279" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A279" s="6" t="s">
         <v>32</v>
       </c>
@@ -18165,7 +18173,7 @@
       <c r="P279" s="6"/>
       <c r="Q279" s="6"/>
     </row>
-    <row r="280" spans="1:17" hidden="1">
+    <row r="280" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A280" s="6" t="s">
         <v>32</v>
       </c>
@@ -18196,7 +18204,7 @@
       <c r="P280" s="6"/>
       <c r="Q280" s="6"/>
     </row>
-    <row r="281" spans="1:17" hidden="1">
+    <row r="281" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A281" s="6" t="s">
         <v>32</v>
       </c>
@@ -18227,7 +18235,7 @@
       <c r="P281" s="6"/>
       <c r="Q281" s="6"/>
     </row>
-    <row r="282" spans="1:17" hidden="1">
+    <row r="282" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A282" s="6" t="s">
         <v>32</v>
       </c>
@@ -18258,7 +18266,7 @@
       <c r="P282" s="6"/>
       <c r="Q282" s="6"/>
     </row>
-    <row r="283" spans="1:17" hidden="1">
+    <row r="283" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A283" s="6" t="s">
         <v>32</v>
       </c>
@@ -18289,7 +18297,7 @@
       <c r="P283" s="6"/>
       <c r="Q283" s="6"/>
     </row>
-    <row r="284" spans="1:17" hidden="1">
+    <row r="284" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A284" s="6" t="s">
         <v>32</v>
       </c>
@@ -18320,7 +18328,7 @@
       <c r="P284" s="6"/>
       <c r="Q284" s="6"/>
     </row>
-    <row r="285" spans="1:17" hidden="1">
+    <row r="285" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A285" s="6" t="s">
         <v>32</v>
       </c>
@@ -18351,7 +18359,7 @@
       <c r="P285" s="6"/>
       <c r="Q285" s="6"/>
     </row>
-    <row r="286" spans="1:17" hidden="1">
+    <row r="286" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A286" s="6" t="s">
         <v>32</v>
       </c>
@@ -18382,7 +18390,7 @@
       <c r="P286" s="6"/>
       <c r="Q286" s="6"/>
     </row>
-    <row r="287" spans="1:17" hidden="1">
+    <row r="287" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A287" s="6" t="s">
         <v>32</v>
       </c>
@@ -18413,7 +18421,7 @@
       <c r="P287" s="6"/>
       <c r="Q287" s="6"/>
     </row>
-    <row r="288" spans="1:17" hidden="1">
+    <row r="288" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A288" s="6" t="s">
         <v>32</v>
       </c>
@@ -18444,7 +18452,7 @@
       <c r="P288" s="6"/>
       <c r="Q288" s="6"/>
     </row>
-    <row r="289" spans="1:17" hidden="1">
+    <row r="289" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A289" s="6" t="s">
         <v>32</v>
       </c>
@@ -18475,7 +18483,7 @@
       <c r="P289" s="6"/>
       <c r="Q289" s="6"/>
     </row>
-    <row r="290" spans="1:17" hidden="1">
+    <row r="290" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A290" s="6" t="s">
         <v>32</v>
       </c>
@@ -18506,7 +18514,7 @@
       <c r="P290" s="6"/>
       <c r="Q290" s="6"/>
     </row>
-    <row r="291" spans="1:17" hidden="1">
+    <row r="291" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A291" s="6" t="s">
         <v>32</v>
       </c>
@@ -18537,7 +18545,7 @@
       <c r="P291" s="6"/>
       <c r="Q291" s="6"/>
     </row>
-    <row r="292" spans="1:17" hidden="1">
+    <row r="292" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A292" s="6" t="s">
         <v>32</v>
       </c>
@@ -18568,7 +18576,7 @@
       <c r="P292" s="6"/>
       <c r="Q292" s="6"/>
     </row>
-    <row r="293" spans="1:17" hidden="1">
+    <row r="293" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A293" s="6" t="s">
         <v>32</v>
       </c>
@@ -18599,7 +18607,7 @@
       <c r="P293" s="6"/>
       <c r="Q293" s="6"/>
     </row>
-    <row r="294" spans="1:17" hidden="1">
+    <row r="294" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A294" s="6" t="s">
         <v>32</v>
       </c>
@@ -18630,7 +18638,7 @@
       <c r="P294" s="6"/>
       <c r="Q294" s="6"/>
     </row>
-    <row r="295" spans="1:17" hidden="1">
+    <row r="295" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A295" s="6" t="s">
         <v>32</v>
       </c>
@@ -18661,7 +18669,7 @@
       <c r="P295" s="6"/>
       <c r="Q295" s="6"/>
     </row>
-    <row r="296" spans="1:17" hidden="1">
+    <row r="296" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A296" s="6" t="s">
         <v>32</v>
       </c>
@@ -18692,7 +18700,7 @@
       <c r="P296" s="6"/>
       <c r="Q296" s="6"/>
     </row>
-    <row r="297" spans="1:17" hidden="1">
+    <row r="297" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A297" s="6" t="s">
         <v>32</v>
       </c>
@@ -18723,7 +18731,7 @@
       <c r="P297" s="6"/>
       <c r="Q297" s="6"/>
     </row>
-    <row r="298" spans="1:17" hidden="1">
+    <row r="298" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A298" s="6" t="s">
         <v>32</v>
       </c>
@@ -18754,7 +18762,7 @@
       <c r="P298" s="6"/>
       <c r="Q298" s="6"/>
     </row>
-    <row r="299" spans="1:17" hidden="1">
+    <row r="299" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A299" s="6" t="s">
         <v>32</v>
       </c>
@@ -18785,7 +18793,7 @@
       <c r="P299" s="6"/>
       <c r="Q299" s="6"/>
     </row>
-    <row r="300" spans="1:17" hidden="1">
+    <row r="300" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A300" s="6" t="s">
         <v>32</v>
       </c>
@@ -18816,7 +18824,7 @@
       <c r="P300" s="6"/>
       <c r="Q300" s="6"/>
     </row>
-    <row r="301" spans="1:17" hidden="1">
+    <row r="301" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A301" s="6" t="s">
         <v>32</v>
       </c>
@@ -18847,7 +18855,7 @@
       <c r="P301" s="6"/>
       <c r="Q301" s="6"/>
     </row>
-    <row r="302" spans="1:17" hidden="1">
+    <row r="302" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A302" s="6" t="s">
         <v>32</v>
       </c>
@@ -18878,7 +18886,7 @@
       <c r="P302" s="6"/>
       <c r="Q302" s="6"/>
     </row>
-    <row r="303" spans="1:17" hidden="1">
+    <row r="303" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A303" s="6" t="s">
         <v>32</v>
       </c>
@@ -18909,7 +18917,7 @@
       <c r="P303" s="6"/>
       <c r="Q303" s="6"/>
     </row>
-    <row r="304" spans="1:17" hidden="1">
+    <row r="304" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A304" s="6" t="s">
         <v>32</v>
       </c>
@@ -18940,7 +18948,7 @@
       <c r="P304" s="6"/>
       <c r="Q304" s="6"/>
     </row>
-    <row r="305" spans="1:17" hidden="1">
+    <row r="305" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A305" s="6" t="s">
         <v>32</v>
       </c>
@@ -18971,7 +18979,7 @@
       <c r="P305" s="6"/>
       <c r="Q305" s="6"/>
     </row>
-    <row r="306" spans="1:17" hidden="1">
+    <row r="306" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A306" s="6" t="s">
         <v>32</v>
       </c>
@@ -19002,7 +19010,7 @@
       <c r="P306" s="6"/>
       <c r="Q306" s="6"/>
     </row>
-    <row r="307" spans="1:17" hidden="1">
+    <row r="307" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A307" s="6" t="s">
         <v>32</v>
       </c>
@@ -19033,7 +19041,7 @@
       <c r="P307" s="6"/>
       <c r="Q307" s="6"/>
     </row>
-    <row r="308" spans="1:17" hidden="1">
+    <row r="308" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A308" s="6" t="s">
         <v>32</v>
       </c>
@@ -19064,7 +19072,7 @@
       <c r="P308" s="6"/>
       <c r="Q308" s="6"/>
     </row>
-    <row r="309" spans="1:17" hidden="1">
+    <row r="309" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A309" s="6" t="s">
         <v>32</v>
       </c>
@@ -19095,7 +19103,7 @@
       <c r="P309" s="6"/>
       <c r="Q309" s="6"/>
     </row>
-    <row r="310" spans="1:17" hidden="1">
+    <row r="310" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A310" s="6" t="s">
         <v>32</v>
       </c>
@@ -19126,7 +19134,7 @@
       <c r="P310" s="6"/>
       <c r="Q310" s="6"/>
     </row>
-    <row r="311" spans="1:17" hidden="1">
+    <row r="311" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A311" s="6" t="s">
         <v>32</v>
       </c>
@@ -19157,7 +19165,7 @@
       <c r="P311" s="6"/>
       <c r="Q311" s="6"/>
     </row>
-    <row r="312" spans="1:17" hidden="1">
+    <row r="312" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A312" s="6" t="s">
         <v>32</v>
       </c>
@@ -19188,7 +19196,7 @@
       <c r="P312" s="6"/>
       <c r="Q312" s="6"/>
     </row>
-    <row r="313" spans="1:17" hidden="1">
+    <row r="313" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A313" s="6" t="s">
         <v>32</v>
       </c>
@@ -19219,7 +19227,7 @@
       <c r="P313" s="6"/>
       <c r="Q313" s="6"/>
     </row>
-    <row r="314" spans="1:17" hidden="1">
+    <row r="314" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A314" s="6" t="s">
         <v>32</v>
       </c>
@@ -19250,7 +19258,7 @@
       <c r="P314" s="6"/>
       <c r="Q314" s="6"/>
     </row>
-    <row r="315" spans="1:17" hidden="1">
+    <row r="315" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A315" s="6" t="s">
         <v>32</v>
       </c>
@@ -19281,7 +19289,7 @@
       <c r="P315" s="6"/>
       <c r="Q315" s="6"/>
     </row>
-    <row r="316" spans="1:17" hidden="1">
+    <row r="316" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A316" s="6" t="s">
         <v>32</v>
       </c>
@@ -19312,7 +19320,7 @@
       <c r="P316" s="6"/>
       <c r="Q316" s="6"/>
     </row>
-    <row r="317" spans="1:17" hidden="1">
+    <row r="317" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A317" s="6" t="s">
         <v>32</v>
       </c>
@@ -19343,7 +19351,7 @@
       <c r="P317" s="6"/>
       <c r="Q317" s="6"/>
     </row>
-    <row r="318" spans="1:17" hidden="1">
+    <row r="318" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A318" s="6" t="s">
         <v>32</v>
       </c>
@@ -19374,7 +19382,7 @@
       <c r="P318" s="6"/>
       <c r="Q318" s="6"/>
     </row>
-    <row r="319" spans="1:17" hidden="1">
+    <row r="319" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A319" s="6" t="s">
         <v>32</v>
       </c>
@@ -19405,7 +19413,7 @@
       <c r="P319" s="6"/>
       <c r="Q319" s="6"/>
     </row>
-    <row r="320" spans="1:17" hidden="1">
+    <row r="320" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A320" s="6" t="s">
         <v>32</v>
       </c>
@@ -19436,7 +19444,7 @@
       <c r="P320" s="6"/>
       <c r="Q320" s="6"/>
     </row>
-    <row r="321" spans="1:17" hidden="1">
+    <row r="321" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A321" s="6" t="s">
         <v>32</v>
       </c>
@@ -19467,7 +19475,7 @@
       <c r="P321" s="6"/>
       <c r="Q321" s="6"/>
     </row>
-    <row r="322" spans="1:17" hidden="1">
+    <row r="322" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A322" s="6" t="s">
         <v>32</v>
       </c>
@@ -19498,7 +19506,7 @@
       <c r="P322" s="6"/>
       <c r="Q322" s="6"/>
     </row>
-    <row r="323" spans="1:17" hidden="1">
+    <row r="323" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A323" s="6" t="s">
         <v>32</v>
       </c>
@@ -19529,7 +19537,7 @@
       <c r="P323" s="6"/>
       <c r="Q323" s="6"/>
     </row>
-    <row r="324" spans="1:17" hidden="1">
+    <row r="324" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A324" s="6" t="s">
         <v>32</v>
       </c>
@@ -19560,7 +19568,7 @@
       <c r="P324" s="6"/>
       <c r="Q324" s="6"/>
     </row>
-    <row r="325" spans="1:17" hidden="1">
+    <row r="325" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A325" s="6" t="s">
         <v>32</v>
       </c>
@@ -19591,7 +19599,7 @@
       <c r="P325" s="6"/>
       <c r="Q325" s="6"/>
     </row>
-    <row r="326" spans="1:17" hidden="1">
+    <row r="326" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A326" s="6" t="s">
         <v>32</v>
       </c>
@@ -19622,7 +19630,7 @@
       <c r="P326" s="6"/>
       <c r="Q326" s="6"/>
     </row>
-    <row r="327" spans="1:17" hidden="1">
+    <row r="327" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A327" s="6" t="s">
         <v>32</v>
       </c>
@@ -19653,7 +19661,7 @@
       <c r="P327" s="6"/>
       <c r="Q327" s="6"/>
     </row>
-    <row r="328" spans="1:17" hidden="1">
+    <row r="328" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A328" s="6" t="s">
         <v>32</v>
       </c>
@@ -19684,7 +19692,7 @@
       <c r="P328" s="6"/>
       <c r="Q328" s="6"/>
     </row>
-    <row r="329" spans="1:17" hidden="1">
+    <row r="329" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A329" s="6" t="s">
         <v>32</v>
       </c>
@@ -19715,7 +19723,7 @@
       <c r="P329" s="6"/>
       <c r="Q329" s="6"/>
     </row>
-    <row r="330" spans="1:17" hidden="1">
+    <row r="330" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A330" s="6" t="s">
         <v>32</v>
       </c>
@@ -19746,7 +19754,7 @@
       <c r="P330" s="6"/>
       <c r="Q330" s="6"/>
     </row>
-    <row r="331" spans="1:17" hidden="1">
+    <row r="331" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A331" s="6" t="s">
         <v>32</v>
       </c>
@@ -19777,7 +19785,7 @@
       <c r="P331" s="6"/>
       <c r="Q331" s="6"/>
     </row>
-    <row r="332" spans="1:17" hidden="1">
+    <row r="332" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A332" s="6" t="s">
         <v>32</v>
       </c>
@@ -19808,7 +19816,7 @@
       <c r="P332" s="6"/>
       <c r="Q332" s="6"/>
     </row>
-    <row r="333" spans="1:17" hidden="1">
+    <row r="333" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A333" s="6" t="s">
         <v>32</v>
       </c>
@@ -19839,7 +19847,7 @@
       <c r="P333" s="6"/>
       <c r="Q333" s="6"/>
     </row>
-    <row r="334" spans="1:17" hidden="1">
+    <row r="334" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A334" s="6" t="s">
         <v>32</v>
       </c>
@@ -19870,7 +19878,7 @@
       <c r="P334" s="6"/>
       <c r="Q334" s="6"/>
     </row>
-    <row r="335" spans="1:17" hidden="1">
+    <row r="335" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A335" s="6" t="s">
         <v>32</v>
       </c>
@@ -19901,7 +19909,7 @@
       <c r="P335" s="6"/>
       <c r="Q335" s="6"/>
     </row>
-    <row r="336" spans="1:17" hidden="1">
+    <row r="336" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A336" s="6" t="s">
         <v>32</v>
       </c>
@@ -19932,7 +19940,7 @@
       <c r="P336" s="6"/>
       <c r="Q336" s="6"/>
     </row>
-    <row r="337" spans="1:17" hidden="1">
+    <row r="337" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A337" s="6" t="s">
         <v>32</v>
       </c>
@@ -19963,7 +19971,7 @@
       <c r="P337" s="6"/>
       <c r="Q337" s="6"/>
     </row>
-    <row r="338" spans="1:17" hidden="1">
+    <row r="338" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A338" s="6" t="s">
         <v>32</v>
       </c>
@@ -19994,7 +20002,7 @@
       <c r="P338" s="6"/>
       <c r="Q338" s="6"/>
     </row>
-    <row r="339" spans="1:17" hidden="1">
+    <row r="339" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A339" s="6" t="s">
         <v>32</v>
       </c>
@@ -20025,7 +20033,7 @@
       <c r="P339" s="6"/>
       <c r="Q339" s="6"/>
     </row>
-    <row r="340" spans="1:17" hidden="1">
+    <row r="340" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A340" s="6" t="s">
         <v>32</v>
       </c>
@@ -20056,7 +20064,7 @@
       <c r="P340" s="6"/>
       <c r="Q340" s="6"/>
     </row>
-    <row r="341" spans="1:17" hidden="1">
+    <row r="341" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A341" s="6" t="s">
         <v>32</v>
       </c>
@@ -20087,7 +20095,7 @@
       <c r="P341" s="6"/>
       <c r="Q341" s="6"/>
     </row>
-    <row r="342" spans="1:17" hidden="1">
+    <row r="342" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A342" s="6" t="s">
         <v>32</v>
       </c>
@@ -20118,7 +20126,7 @@
       <c r="P342" s="6"/>
       <c r="Q342" s="6"/>
     </row>
-    <row r="343" spans="1:17" hidden="1">
+    <row r="343" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A343" s="6" t="s">
         <v>32</v>
       </c>
@@ -20149,7 +20157,7 @@
       <c r="P343" s="6"/>
       <c r="Q343" s="6"/>
     </row>
-    <row r="344" spans="1:17" hidden="1">
+    <row r="344" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A344" s="6" t="s">
         <v>32</v>
       </c>
@@ -20180,7 +20188,7 @@
       <c r="P344" s="6"/>
       <c r="Q344" s="6"/>
     </row>
-    <row r="345" spans="1:17" hidden="1">
+    <row r="345" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A345" s="6" t="s">
         <v>32</v>
       </c>
@@ -20211,7 +20219,7 @@
       <c r="P345" s="6"/>
       <c r="Q345" s="6"/>
     </row>
-    <row r="346" spans="1:17" hidden="1">
+    <row r="346" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A346" s="6" t="s">
         <v>32</v>
       </c>
@@ -20242,7 +20250,7 @@
       <c r="P346" s="6"/>
       <c r="Q346" s="6"/>
     </row>
-    <row r="347" spans="1:17" hidden="1">
+    <row r="347" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A347" s="6" t="s">
         <v>32</v>
       </c>
@@ -20273,7 +20281,7 @@
       <c r="P347" s="6"/>
       <c r="Q347" s="6"/>
     </row>
-    <row r="348" spans="1:17" hidden="1">
+    <row r="348" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A348" s="6" t="s">
         <v>32</v>
       </c>
@@ -20304,7 +20312,7 @@
       <c r="P348" s="6"/>
       <c r="Q348" s="6"/>
     </row>
-    <row r="349" spans="1:17" hidden="1">
+    <row r="349" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A349" s="6" t="s">
         <v>32</v>
       </c>
@@ -20335,7 +20343,7 @@
       <c r="P349" s="6"/>
       <c r="Q349" s="6"/>
     </row>
-    <row r="350" spans="1:17" hidden="1">
+    <row r="350" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A350" s="6" t="s">
         <v>32</v>
       </c>
@@ -20366,7 +20374,7 @@
       <c r="P350" s="6"/>
       <c r="Q350" s="6"/>
     </row>
-    <row r="351" spans="1:17" hidden="1">
+    <row r="351" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A351" s="6" t="s">
         <v>32</v>
       </c>
@@ -20397,7 +20405,7 @@
       <c r="P351" s="6"/>
       <c r="Q351" s="6"/>
     </row>
-    <row r="352" spans="1:17" hidden="1">
+    <row r="352" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A352" s="6" t="s">
         <v>32</v>
       </c>
@@ -20428,7 +20436,7 @@
       <c r="P352" s="6"/>
       <c r="Q352" s="6"/>
     </row>
-    <row r="353" spans="1:17" hidden="1">
+    <row r="353" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A353" s="6" t="s">
         <v>32</v>
       </c>
@@ -20459,7 +20467,7 @@
       <c r="P353" s="6"/>
       <c r="Q353" s="6"/>
     </row>
-    <row r="354" spans="1:17" hidden="1">
+    <row r="354" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A354" s="6" t="s">
         <v>32</v>
       </c>
@@ -20490,7 +20498,7 @@
       <c r="P354" s="6"/>
       <c r="Q354" s="6"/>
     </row>
-    <row r="355" spans="1:17" hidden="1">
+    <row r="355" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A355" s="6" t="s">
         <v>32</v>
       </c>
@@ -20521,7 +20529,7 @@
       <c r="P355" s="6"/>
       <c r="Q355" s="6"/>
     </row>
-    <row r="356" spans="1:17" hidden="1">
+    <row r="356" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A356" s="6" t="s">
         <v>32</v>
       </c>
@@ -20552,7 +20560,7 @@
       <c r="P356" s="6"/>
       <c r="Q356" s="6"/>
     </row>
-    <row r="357" spans="1:17" hidden="1">
+    <row r="357" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A357" s="6" t="s">
         <v>32</v>
       </c>
@@ -20583,7 +20591,7 @@
       <c r="P357" s="6"/>
       <c r="Q357" s="6"/>
     </row>
-    <row r="358" spans="1:17" hidden="1">
+    <row r="358" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A358" s="6" t="s">
         <v>32</v>
       </c>
@@ -20614,7 +20622,7 @@
       <c r="P358" s="6"/>
       <c r="Q358" s="6"/>
     </row>
-    <row r="359" spans="1:17" hidden="1">
+    <row r="359" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A359" s="6" t="s">
         <v>32</v>
       </c>
@@ -20645,7 +20653,7 @@
       <c r="P359" s="6"/>
       <c r="Q359" s="6"/>
     </row>
-    <row r="360" spans="1:17" hidden="1">
+    <row r="360" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A360" s="6" t="s">
         <v>32</v>
       </c>
@@ -20676,7 +20684,7 @@
       <c r="P360" s="6"/>
       <c r="Q360" s="6"/>
     </row>
-    <row r="361" spans="1:17" hidden="1">
+    <row r="361" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A361" s="6" t="s">
         <v>32</v>
       </c>
@@ -20707,7 +20715,7 @@
       <c r="P361" s="6"/>
       <c r="Q361" s="6"/>
     </row>
-    <row r="362" spans="1:17" hidden="1">
+    <row r="362" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A362" s="6" t="s">
         <v>32</v>
       </c>
@@ -20738,7 +20746,7 @@
       <c r="P362" s="6"/>
       <c r="Q362" s="6"/>
     </row>
-    <row r="363" spans="1:17" hidden="1">
+    <row r="363" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A363" s="6" t="s">
         <v>32</v>
       </c>
@@ -20769,7 +20777,7 @@
       <c r="P363" s="6"/>
       <c r="Q363" s="6"/>
     </row>
-    <row r="364" spans="1:17" hidden="1">
+    <row r="364" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A364" s="6" t="s">
         <v>32</v>
       </c>
@@ -20800,7 +20808,7 @@
       <c r="P364" s="6"/>
       <c r="Q364" s="6"/>
     </row>
-    <row r="365" spans="1:17" hidden="1">
+    <row r="365" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A365" s="6" t="s">
         <v>32</v>
       </c>
@@ -20831,7 +20839,7 @@
       <c r="P365" s="6"/>
       <c r="Q365" s="6"/>
     </row>
-    <row r="366" spans="1:17" hidden="1">
+    <row r="366" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A366" s="6" t="s">
         <v>32</v>
       </c>
@@ -20862,7 +20870,7 @@
       <c r="P366" s="6"/>
       <c r="Q366" s="6"/>
     </row>
-    <row r="367" spans="1:17" hidden="1">
+    <row r="367" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A367" s="6" t="s">
         <v>32</v>
       </c>
@@ -20893,7 +20901,7 @@
       <c r="P367" s="6"/>
       <c r="Q367" s="6"/>
     </row>
-    <row r="368" spans="1:17" hidden="1">
+    <row r="368" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A368" s="6" t="s">
         <v>32</v>
       </c>
@@ -20924,7 +20932,7 @@
       <c r="P368" s="6"/>
       <c r="Q368" s="6"/>
     </row>
-    <row r="369" spans="1:17" hidden="1">
+    <row r="369" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A369" s="6" t="s">
         <v>32</v>
       </c>
@@ -20955,7 +20963,7 @@
       <c r="P369" s="6"/>
       <c r="Q369" s="6"/>
     </row>
-    <row r="370" spans="1:17" hidden="1">
+    <row r="370" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A370" s="6" t="s">
         <v>32</v>
       </c>
@@ -20986,7 +20994,7 @@
       <c r="P370" s="6"/>
       <c r="Q370" s="6"/>
     </row>
-    <row r="371" spans="1:17" hidden="1">
+    <row r="371" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A371" s="6" t="s">
         <v>32</v>
       </c>
@@ -21017,7 +21025,7 @@
       <c r="P371" s="6"/>
       <c r="Q371" s="6"/>
     </row>
-    <row r="372" spans="1:17" hidden="1">
+    <row r="372" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A372" s="6" t="s">
         <v>32</v>
       </c>
@@ -21048,7 +21056,7 @@
       <c r="P372" s="6"/>
       <c r="Q372" s="6"/>
     </row>
-    <row r="373" spans="1:17" hidden="1">
+    <row r="373" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A373" s="6" t="s">
         <v>32</v>
       </c>
@@ -21079,7 +21087,7 @@
       <c r="P373" s="6"/>
       <c r="Q373" s="6"/>
     </row>
-    <row r="374" spans="1:17" ht="29" hidden="1">
+    <row r="374" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A374" s="6" t="s">
         <v>32</v>
       </c>
@@ -21110,7 +21118,7 @@
       <c r="P374" s="6"/>
       <c r="Q374" s="6"/>
     </row>
-    <row r="375" spans="1:17" ht="29" hidden="1">
+    <row r="375" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A375" s="6" t="s">
         <v>32</v>
       </c>
@@ -21141,7 +21149,7 @@
       <c r="P375" s="6"/>
       <c r="Q375" s="6"/>
     </row>
-    <row r="376" spans="1:17" ht="43.5">
+    <row r="376" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A376" s="6" t="s">
         <v>32</v>
       </c>
@@ -21176,14 +21184,70 @@
       <c r="P376" s="6"/>
       <c r="Q376" s="6"/>
     </row>
+    <row r="377" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+      <c r="A377" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B377" s="6" t="s">
+        <v>626</v>
+      </c>
+      <c r="C377" s="6" t="s">
+        <v>1601</v>
+      </c>
+      <c r="D377" s="6" t="s">
+        <v>1600</v>
+      </c>
+      <c r="E377" s="6"/>
+      <c r="F377" s="6"/>
+      <c r="G377" s="6"/>
+      <c r="H377" s="6"/>
+      <c r="I377" s="6"/>
+      <c r="J377" s="6"/>
+      <c r="K377" s="6"/>
+      <c r="L377" s="6" t="s">
+        <v>644</v>
+      </c>
+      <c r="M377" s="6" t="s">
+        <v>645</v>
+      </c>
+      <c r="N377" s="6"/>
+      <c r="O377" s="6"/>
+      <c r="P377" s="6"/>
+      <c r="Q377" s="6"/>
+    </row>
+    <row r="378" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A378" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B378" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="C378" s="6" t="s">
+        <v>1602</v>
+      </c>
+      <c r="D378" s="6" t="s">
+        <v>1600</v>
+      </c>
+      <c r="E378" s="6"/>
+      <c r="F378" s="6"/>
+      <c r="G378" s="6"/>
+      <c r="H378" s="6"/>
+      <c r="I378" s="6"/>
+      <c r="J378" s="6"/>
+      <c r="K378" s="6"/>
+      <c r="L378" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="M378" s="6" t="s">
+        <v>420</v>
+      </c>
+      <c r="N378" s="6"/>
+      <c r="O378" s="6"/>
+      <c r="P378" s="6"/>
+      <c r="Q378" s="6"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:Q376" xr:uid="{00000000-0009-0000-0000-000001000000}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="Labo"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:Q378" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="N169" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>

</xml_diff>